<commit_message>
Screening functions added and some renaming
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cm1om\Documents\Research\Cancer\Bladder\Bladder_cancer_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB06D3F-CDA4-468F-AF87-59E887018B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E749D9-1348-4A8D-94BD-BF04E642F58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1AD6D928-CCB7-482A-A47C-26785A7D3A52}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1AD6D928-CCB7-482A-A47C-26785A7D3A52}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3214" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3209" uniqueCount="344">
   <si>
     <t>Param number</t>
   </si>
@@ -1115,13 +1115,7 @@
     <t>Sensitivity of flexible cystoscopy (all stages HG)</t>
   </si>
   <si>
-    <t>Specificity of  flexible cystoscopy (all stages HG)</t>
-  </si>
-  <si>
     <t>Sensitivity of flexible cystoscopy (LG)</t>
-  </si>
-  <si>
-    <t>Specificity of  flexible cystoscopy (LG)</t>
   </si>
   <si>
     <r>
@@ -1215,13 +1209,7 @@
     <t>Sens.cystoscopy.HG</t>
   </si>
   <si>
-    <t>Spec.cystoscopy.HG</t>
-  </si>
-  <si>
     <t>Sens.cystoscopy.LG</t>
-  </si>
-  <si>
-    <t>Spec.cystoscopy.LG</t>
   </si>
   <si>
     <t>Harms</t>
@@ -1454,6 +1442,12 @@
   </si>
   <si>
     <t>uniform</t>
+  </si>
+  <si>
+    <t>Specificity of  flexible cystoscopy</t>
+  </si>
+  <si>
+    <t>Spec.cystoscopy</t>
   </si>
 </sst>
 </file>
@@ -3571,10 +3565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8694223C-410D-4023-9128-3FD5F8A481E4}">
-  <dimension ref="A1:Z70"/>
+  <dimension ref="A1:Z69"/>
   <sheetViews>
-    <sheetView topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3624,7 +3618,7 @@
       </c>
       <c r="I1" s="115"/>
       <c r="J1" s="105" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="K1" s="116" t="s">
         <v>6</v>
@@ -3661,7 +3655,7 @@
         <v>9.8400000000000007E-6</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G2" s="5">
         <v>7</v>
@@ -3679,7 +3673,7 @@
         <v>0.01</v>
       </c>
       <c r="N2" s="68" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="O2" s="95"/>
       <c r="P2" s="68">
@@ -3724,7 +3718,7 @@
         <v>0.65200000000000002</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G3" s="5">
         <v>7</v>
@@ -3742,7 +3736,7 @@
         <v>0.05</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="O3" s="96" t="s">
         <v>36</v>
@@ -3790,7 +3784,7 @@
         <v>1.99</v>
       </c>
       <c r="F4" s="68" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G4" s="68">
         <v>3</v>
@@ -3852,7 +3846,7 @@
         <v>2.1744970000000001</v>
       </c>
       <c r="F5" s="68" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G5" s="68">
         <v>3</v>
@@ -3922,7 +3916,7 @@
         <v>5.9977460000000002</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G6" s="68">
         <v>3</v>
@@ -3975,7 +3969,7 @@
         <v>1.2</v>
       </c>
       <c r="F7" s="68" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G7" s="68">
         <v>3</v>
@@ -4022,7 +4016,7 @@
         <v>2.76</v>
       </c>
       <c r="F8" s="68" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G8" s="68">
         <v>3</v>
@@ -4069,7 +4063,7 @@
         <v>1.67E-2</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G9" s="5">
         <v>7</v>
@@ -4116,7 +4110,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="F10" s="106" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G10" s="106">
         <v>5</v>
@@ -4156,7 +4150,7 @@
         <v>3.75</v>
       </c>
       <c r="F11" s="106" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G11" s="106">
         <v>5</v>
@@ -4199,7 +4193,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G12" s="5">
         <v>7</v>
@@ -4228,17 +4222,17 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D13" s="68" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E13" s="110">
         <f>H13</f>
         <v>0.121</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G13" s="5">
         <v>7</v>
@@ -4264,17 +4258,17 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D14" s="68" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E14" s="110">
         <f t="shared" ref="E14:E15" si="2">H14</f>
         <v>0.22700000000000001</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G14" s="5">
         <v>7</v>
@@ -4301,17 +4295,17 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D15" s="68" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E15" s="110">
         <f t="shared" si="2"/>
         <v>0.876</v>
       </c>
       <c r="F15" s="106" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G15" s="106">
         <v>5</v>
@@ -4347,7 +4341,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G16" s="5">
         <v>4</v>
@@ -4380,7 +4374,7 @@
         <v>3</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G17" s="5">
         <v>6</v>
@@ -4419,7 +4413,7 @@
         <v>2</v>
       </c>
       <c r="F18" s="68" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G18" s="68">
         <v>6</v>
@@ -4455,7 +4449,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="68" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G19" s="68">
         <v>6</v>
@@ -4492,7 +4486,7 @@
         <v>0.75472189999999995</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G20" s="5">
         <v>5</v>
@@ -4539,7 +4533,7 @@
         <v>0.66200000000000003</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G21" s="5">
         <v>7</v>
@@ -4577,7 +4571,7 @@
         <v>0.76600000000000001</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G22" s="5">
         <v>7</v>
@@ -4614,7 +4608,7 @@
         <v>0.42299999999999999</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G23" s="5">
         <v>7</v>
@@ -4641,7 +4635,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>78</v>
@@ -4651,7 +4645,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G24" s="5">
         <v>7</v>
@@ -4697,7 +4691,7 @@
         <v>0.28499999999999998</v>
       </c>
       <c r="F25" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G25" s="68">
         <v>5</v>
@@ -4735,17 +4729,17 @@
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D26" s="106" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E26" s="111">
         <f>H26</f>
         <v>0.91200000000000003</v>
       </c>
       <c r="F26" s="106" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G26" s="106">
         <v>5</v>
@@ -4770,13 +4764,13 @@
         <v>222</v>
       </c>
       <c r="D27" s="68" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E27" s="68">
         <v>0.70957585397710221</v>
       </c>
       <c r="F27" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G27" s="68">
         <v>5</v>
@@ -4790,7 +4784,7 @@
         <v>4.4760529439603229E-2</v>
       </c>
       <c r="J27" s="106">
-        <f t="shared" ref="J27:J70" si="7">E27</f>
+        <f t="shared" ref="J27:J69" si="7">E27</f>
         <v>0.70957585397710221</v>
       </c>
       <c r="K27" s="68">
@@ -4811,13 +4805,13 @@
         <v>223</v>
       </c>
       <c r="D28" s="68" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E28" s="68">
         <v>-0.36468752598392556</v>
       </c>
       <c r="F28" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G28" s="68">
         <v>5</v>
@@ -4852,13 +4846,13 @@
         <v>224</v>
       </c>
       <c r="D29" s="68" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E29" s="68">
         <v>-0.25156411279366031</v>
       </c>
       <c r="F29" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G29" s="68">
         <v>5</v>
@@ -4893,13 +4887,13 @@
         <v>225</v>
       </c>
       <c r="D30" s="68" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E30" s="68">
         <v>-0.11653381625595151</v>
       </c>
       <c r="F30" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G30" s="68">
         <v>5</v>
@@ -4934,13 +4928,13 @@
         <v>226</v>
       </c>
       <c r="D31" s="68" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E31" s="68">
         <v>-0.23572233352106983</v>
       </c>
       <c r="F31" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G31" s="68">
         <v>5</v>
@@ -4975,13 +4969,13 @@
         <v>227</v>
       </c>
       <c r="D32" s="68" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E32" s="68">
         <v>0.13976194237515863</v>
       </c>
       <c r="F32" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G32" s="68">
         <v>5</v>
@@ -5016,13 +5010,13 @@
         <v>228</v>
       </c>
       <c r="D33" s="68" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E33" s="68">
         <v>-1.8325814637483102</v>
       </c>
       <c r="F33" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G33" s="68">
         <v>5</v>
@@ -5054,16 +5048,16 @@
         <v>218</v>
       </c>
       <c r="C34" s="104" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D34" s="104" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E34" s="104">
         <v>1.8794650496471605</v>
       </c>
       <c r="F34" s="104" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G34" s="104">
         <v>5</v>
@@ -5098,13 +5092,13 @@
         <v>229</v>
       </c>
       <c r="D35" s="68" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E35" s="68">
         <v>-7.2570692834835374E-2</v>
       </c>
       <c r="F35" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G35" s="68">
         <v>5</v>
@@ -5139,13 +5133,13 @@
         <v>230</v>
       </c>
       <c r="D36" s="68" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E36" s="68">
         <v>-0.15082288973458366</v>
       </c>
       <c r="F36" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G36" s="68">
         <v>5</v>
@@ -5180,13 +5174,13 @@
         <v>231</v>
       </c>
       <c r="D37" s="68" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E37" s="68">
         <v>-0.2876820724517809</v>
       </c>
       <c r="F37" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G37" s="68">
         <v>5</v>
@@ -5221,13 +5215,13 @@
         <v>232</v>
       </c>
       <c r="D38" s="68" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E38" s="68">
         <v>-0.59783700075562041</v>
       </c>
       <c r="F38" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G38" s="68">
         <v>5</v>
@@ -5262,13 +5256,13 @@
         <v>233</v>
       </c>
       <c r="D39" s="68" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E39" s="68">
         <v>-0.94057230424574823</v>
       </c>
       <c r="F39" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G39" s="68">
         <v>5</v>
@@ -5303,7 +5297,7 @@
         <v>234</v>
       </c>
       <c r="D40" s="68" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E40" s="68">
         <v>1</v>
@@ -5334,7 +5328,7 @@
         <v>242</v>
       </c>
       <c r="D41" s="68" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E41" s="97">
         <v>0.23</v>
@@ -5376,7 +5370,7 @@
         <v>82</v>
       </c>
       <c r="D42" s="68" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E42" s="97">
         <v>0.5</v>
@@ -5418,7 +5412,7 @@
         <v>238</v>
       </c>
       <c r="D43" s="68" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E43" s="97">
         <v>0.88</v>
@@ -5460,7 +5454,7 @@
         <v>239</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E44" s="108">
         <v>0.82</v>
@@ -5490,10 +5484,10 @@
         <v>0.93</v>
       </c>
       <c r="N44" s="109" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="Q44" s="31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="2:19">
@@ -5504,7 +5498,7 @@
         <v>247</v>
       </c>
       <c r="D45" s="68" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E45" s="97">
         <v>0.94299999999999995</v>
@@ -5547,10 +5541,10 @@
         <v>236</v>
       </c>
       <c r="C46" s="99" t="s">
-        <v>248</v>
+        <v>342</v>
       </c>
       <c r="D46" s="68" t="s">
-        <v>274</v>
+        <v>343</v>
       </c>
       <c r="E46" s="97">
         <v>0.84699999999999998</v>
@@ -5594,10 +5588,10 @@
         <v>236</v>
       </c>
       <c r="C47" s="99" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D47" s="68" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E47" s="97">
         <v>0.92700000000000005</v>
@@ -5628,7 +5622,7 @@
         <v>0.94863518192260199</v>
       </c>
       <c r="N47" s="97" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="Q47" s="92">
         <v>0.878</v>
@@ -5640,276 +5634,269 @@
     </row>
     <row r="48" spans="2:19">
       <c r="B48" s="68" t="s">
-        <v>236</v>
-      </c>
-      <c r="C48" s="99" t="s">
-        <v>250</v>
+        <v>273</v>
+      </c>
+      <c r="C48" s="68" t="s">
+        <v>79</v>
       </c>
       <c r="D48" s="68" t="s">
-        <v>276</v>
-      </c>
-      <c r="E48" s="97">
-        <v>0.76800000000000002</v>
+        <v>274</v>
+      </c>
+      <c r="E48" s="68">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F48" s="68" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="G48" s="68">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H48" s="68">
-        <v>719</v>
-      </c>
-      <c r="I48" s="93">
-        <f>H48-H48*E48</f>
-        <v>166.80799999999999</v>
+        <f>E48</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I48" s="100">
+        <f>(L48-K48)/(2*NORMINV(0.975,0,1))</f>
+        <v>2.55106728462327E-3</v>
       </c>
       <c r="J48" s="106">
         <f t="shared" si="7"/>
-        <v>0.76800000000000002</v>
-      </c>
-      <c r="K48" s="92">
-        <f>_xlfn.BETA.INV(0.025,H48,I48)</f>
-        <v>0.78530286018445838</v>
-      </c>
-      <c r="L48" s="92">
-        <f>_xlfn.BETA.INV(0.975,H48,I48)</f>
-        <v>0.83674085794535835</v>
-      </c>
-      <c r="N48" s="97" t="s">
-        <v>251</v>
-      </c>
-      <c r="Q48" s="92">
-        <v>0.73</v>
-      </c>
-      <c r="R48" s="92">
-        <v>0.80200000000000005</v>
-      </c>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K48" s="101">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L48" s="101">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="N48" s="68" t="s">
+        <v>275</v>
+      </c>
+      <c r="O48" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q48" s="92"/>
+      <c r="R48" s="92"/>
       <c r="S48" s="92"/>
     </row>
-    <row r="49" spans="2:19">
+    <row r="49" spans="2:14">
       <c r="B49" s="68" t="s">
-        <v>277</v>
+        <v>26</v>
       </c>
       <c r="C49" s="68" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="D49" s="68" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E49" s="68">
-        <v>8.0000000000000002E-3</v>
+        <v>4.3200000000000001E-3</v>
       </c>
       <c r="F49" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G49" s="68">
         <v>5</v>
       </c>
       <c r="H49" s="68">
         <f>E49</f>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="I49" s="100">
+        <v>4.3200000000000001E-3</v>
+      </c>
+      <c r="I49" s="68">
         <f>(L49-K49)/(2*NORMINV(0.975,0,1))</f>
-        <v>2.55106728462327E-3</v>
+        <v>1.4285976793890307E-4</v>
       </c>
       <c r="J49" s="106">
         <f t="shared" si="7"/>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="K49" s="101">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="L49" s="101">
-        <v>1.2999999999999999E-2</v>
+        <v>4.3200000000000001E-3</v>
+      </c>
+      <c r="K49" s="68">
+        <v>4.0400000000000002E-3</v>
+      </c>
+      <c r="L49" s="68">
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="N49" s="68" t="s">
-        <v>279</v>
-      </c>
-      <c r="O49" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q49" s="92"/>
-      <c r="R49" s="92"/>
-      <c r="S49" s="92"/>
-    </row>
-    <row r="50" spans="2:19">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14">
       <c r="B50" s="68" t="s">
         <v>26</v>
       </c>
       <c r="C50" s="68" t="s">
-        <v>27</v>
+        <v>277</v>
       </c>
       <c r="D50" s="68" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E50" s="68">
-        <v>4.3200000000000001E-3</v>
+        <v>-0.08</v>
       </c>
       <c r="F50" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G50" s="68">
         <v>5</v>
       </c>
       <c r="H50" s="68">
-        <f>E50</f>
-        <v>4.3200000000000001E-3</v>
+        <f t="shared" ref="H50:H52" si="8">E50</f>
+        <v>-0.08</v>
       </c>
       <c r="I50" s="68">
         <f>(L50-K50)/(2*NORMINV(0.975,0,1))</f>
-        <v>1.4285976793890307E-4</v>
+        <v>4.3368143838595594E-2</v>
       </c>
       <c r="J50" s="106">
-        <f t="shared" si="7"/>
-        <v>4.3200000000000001E-3</v>
+        <f>E50</f>
+        <v>-0.08</v>
       </c>
       <c r="K50" s="68">
-        <v>4.0400000000000002E-3</v>
+        <v>-0.3</v>
       </c>
       <c r="L50" s="68">
-        <v>4.5999999999999999E-3</v>
+        <v>-0.13</v>
       </c>
       <c r="N50" s="68" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="51" spans="2:19">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14">
       <c r="B51" s="68" t="s">
         <v>26</v>
       </c>
       <c r="C51" s="68" t="s">
-        <v>281</v>
+        <v>323</v>
       </c>
       <c r="D51" s="68" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E51" s="68">
-        <v>-0.08</v>
+        <v>-0.18</v>
       </c>
       <c r="F51" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G51" s="68">
         <v>5</v>
       </c>
       <c r="H51" s="68">
-        <f t="shared" ref="H51:H53" si="8">E51</f>
-        <v>-0.08</v>
+        <f t="shared" si="8"/>
+        <v>-0.18</v>
       </c>
       <c r="I51" s="68">
         <f>(L51-K51)/(2*NORMINV(0.975,0,1))</f>
-        <v>4.3368143838595594E-2</v>
+        <v>6.1225614830958487E-2</v>
       </c>
       <c r="J51" s="106">
-        <f>E51</f>
-        <v>-0.08</v>
+        <f t="shared" si="7"/>
+        <v>-0.18</v>
       </c>
       <c r="K51" s="68">
         <v>-0.3</v>
       </c>
       <c r="L51" s="68">
-        <v>-0.13</v>
+        <v>-0.06</v>
       </c>
       <c r="N51" s="68" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="52" spans="2:19">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14">
       <c r="B52" s="68" t="s">
         <v>26</v>
       </c>
       <c r="C52" s="68" t="s">
-        <v>327</v>
+        <v>282</v>
       </c>
       <c r="D52" s="68" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E52" s="68">
-        <v>-0.18</v>
+        <v>0</v>
       </c>
       <c r="F52" s="68" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="G52" s="68">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H52" s="68">
         <f t="shared" si="8"/>
-        <v>-0.18</v>
+        <v>0</v>
       </c>
       <c r="I52" s="68">
-        <f>(L52-K52)/(2*NORMINV(0.975,0,1))</f>
-        <v>6.1225614830958487E-2</v>
+        <f t="shared" ref="I52" si="9">(L52-K52)/(2*NORMINV(0.975,0,1))</f>
+        <v>0</v>
       </c>
       <c r="J52" s="106">
         <f t="shared" si="7"/>
-        <v>-0.18</v>
+        <v>0</v>
       </c>
       <c r="K52" s="68">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="L52" s="68">
-        <v>-0.06</v>
+        <v>0</v>
       </c>
       <c r="N52" s="68" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14">
+      <c r="B53" s="68" t="s">
+        <v>284</v>
+      </c>
+      <c r="C53" s="68" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="53" spans="2:19">
-      <c r="B53" s="68" t="s">
-        <v>26</v>
-      </c>
-      <c r="C53" s="68" t="s">
+      <c r="D53" s="68" t="s">
         <v>286</v>
       </c>
-      <c r="D53" s="68" t="s">
-        <v>287</v>
-      </c>
       <c r="E53" s="68">
-        <v>0</v>
+        <v>610.58000000000004</v>
       </c>
       <c r="F53" s="68" t="s">
-        <v>244</v>
+        <v>47</v>
       </c>
       <c r="G53" s="68">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H53" s="68">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I53" s="68">
-        <f t="shared" ref="I53" si="9">(L53-K53)/(2*NORMINV(0.975,0,1))</f>
-        <v>0</v>
+        <f>E53/H53</f>
+        <v>6.1058000000000003</v>
       </c>
       <c r="J53" s="106">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>610.58000000000004</v>
       </c>
       <c r="K53" s="68">
-        <v>0</v>
+        <f>_xlfn.GAMMA.INV(0.025,H53,I53)</f>
+        <v>496.79225777988648</v>
       </c>
       <c r="L53" s="68">
-        <v>0</v>
+        <f>_xlfn.GAMMA.INV(0.975,H53,I53)</f>
+        <v>735.92564919121662</v>
       </c>
       <c r="N53" s="68" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="54" spans="2:19">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14">
       <c r="B54" s="68" t="s">
+        <v>284</v>
+      </c>
+      <c r="C54" s="68" t="s">
         <v>288</v>
       </c>
-      <c r="C54" s="68" t="s">
+      <c r="D54" s="68" t="s">
         <v>289</v>
       </c>
-      <c r="D54" s="68" t="s">
-        <v>290</v>
-      </c>
       <c r="E54" s="68">
-        <v>610.58000000000004</v>
+        <v>584.89</v>
       </c>
       <c r="F54" s="68" t="s">
         <v>47</v>
@@ -5922,36 +5909,36 @@
       </c>
       <c r="I54" s="68">
         <f>E54/H54</f>
-        <v>6.1058000000000003</v>
+        <v>5.8488999999999995</v>
       </c>
       <c r="J54" s="106">
         <f t="shared" si="7"/>
-        <v>610.58000000000004</v>
+        <v>584.89</v>
       </c>
       <c r="K54" s="68">
         <f>_xlfn.GAMMA.INV(0.025,H54,I54)</f>
-        <v>496.79225777988648</v>
+        <v>475.88984842752427</v>
       </c>
       <c r="L54" s="68">
         <f>_xlfn.GAMMA.INV(0.975,H54,I54)</f>
-        <v>735.92564919121662</v>
+        <v>704.96176251343081</v>
       </c>
       <c r="N54" s="68" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14">
+      <c r="B55" s="68" t="s">
+        <v>284</v>
+      </c>
+      <c r="C55" s="68" t="s">
+        <v>290</v>
+      </c>
+      <c r="D55" s="68" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="55" spans="2:19">
-      <c r="B55" s="68" t="s">
-        <v>288</v>
-      </c>
-      <c r="C55" s="68" t="s">
-        <v>292</v>
-      </c>
-      <c r="D55" s="68" t="s">
-        <v>293</v>
-      </c>
       <c r="E55" s="68">
-        <v>584.89</v>
+        <v>2348.8000000000002</v>
       </c>
       <c r="F55" s="68" t="s">
         <v>47</v>
@@ -5964,466 +5951,466 @@
       </c>
       <c r="I55" s="68">
         <f>E55/H55</f>
-        <v>5.8488999999999995</v>
+        <v>23.488000000000003</v>
       </c>
       <c r="J55" s="106">
         <f t="shared" si="7"/>
-        <v>584.89</v>
+        <v>2348.8000000000002</v>
       </c>
       <c r="K55" s="68">
         <f>_xlfn.GAMMA.INV(0.025,H55,I55)</f>
-        <v>475.88984842752427</v>
+        <v>1911.0774265016828</v>
       </c>
       <c r="L55" s="68">
-        <f>_xlfn.GAMMA.INV(0.975,H55,I55)</f>
-        <v>704.96176251343081</v>
-      </c>
+        <f t="shared" ref="L55" si="10">_xlfn.GAMMA.INV(0.975,H55,I55)</f>
+        <v>2830.9839248261155</v>
+      </c>
+      <c r="M55" s="91"/>
       <c r="N55" s="68" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="56" spans="2:19">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14">
       <c r="B56" s="68" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C56" s="68" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D56" s="68" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E56" s="68">
-        <v>2348.8000000000002</v>
+        <v>-57.2</v>
       </c>
       <c r="F56" s="68" t="s">
-        <v>47</v>
+        <v>252</v>
       </c>
       <c r="G56" s="68">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H56" s="68">
-        <v>100</v>
+        <f>E56</f>
+        <v>-57.2</v>
       </c>
       <c r="I56" s="68">
-        <f>E56/H56</f>
-        <v>23.488000000000003</v>
+        <f>-E56*0.1</f>
+        <v>5.7200000000000006</v>
       </c>
       <c r="J56" s="106">
         <f t="shared" si="7"/>
-        <v>2348.8000000000002</v>
+        <v>-57.2</v>
       </c>
       <c r="K56" s="68">
-        <f>_xlfn.GAMMA.INV(0.025,H56,I56)</f>
-        <v>1911.0774265016828</v>
+        <f>E56-(I56*NORMINV(0.975,0,1))</f>
+        <v>-68.410993991569114</v>
       </c>
       <c r="L56" s="68">
-        <f t="shared" ref="L56" si="10">_xlfn.GAMMA.INV(0.975,H56,I56)</f>
-        <v>2830.9839248261155</v>
-      </c>
-      <c r="M56" s="91"/>
+        <f>E56+(I56*NORMINV(0.975,0,1))</f>
+        <v>-45.989006008430891</v>
+      </c>
       <c r="N56" s="68" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="57" spans="2:19">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14">
       <c r="B57" s="68" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C57" s="68" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D57" s="68" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E57" s="68">
-        <v>-57.2</v>
+        <v>-242</v>
       </c>
       <c r="F57" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G57" s="68">
         <v>5</v>
       </c>
       <c r="H57" s="68">
-        <f>E57</f>
-        <v>-57.2</v>
+        <f t="shared" ref="H57:H58" si="11">E57</f>
+        <v>-242</v>
       </c>
       <c r="I57" s="68">
         <f>-E57*0.1</f>
-        <v>5.7200000000000006</v>
+        <v>24.200000000000003</v>
       </c>
       <c r="J57" s="106">
         <f t="shared" si="7"/>
-        <v>-57.2</v>
+        <v>-242</v>
       </c>
       <c r="K57" s="68">
         <f>E57-(I57*NORMINV(0.975,0,1))</f>
-        <v>-68.410993991569114</v>
+        <v>-289.4311284258693</v>
       </c>
       <c r="L57" s="68">
         <f>E57+(I57*NORMINV(0.975,0,1))</f>
-        <v>-45.989006008430891</v>
+        <v>-194.5688715741307</v>
       </c>
       <c r="N57" s="68" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="58" spans="2:19">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14">
       <c r="B58" s="68" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C58" s="68" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D58" s="68" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E58" s="68">
-        <v>-242</v>
+        <v>-921.4</v>
       </c>
       <c r="F58" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G58" s="68">
         <v>5</v>
       </c>
       <c r="H58" s="68">
-        <f t="shared" ref="H58:H59" si="11">E58</f>
-        <v>-242</v>
+        <f t="shared" si="11"/>
+        <v>-921.4</v>
       </c>
       <c r="I58" s="68">
         <f>-E58*0.1</f>
-        <v>24.200000000000003</v>
+        <v>92.14</v>
       </c>
       <c r="J58" s="106">
-        <f t="shared" si="7"/>
-        <v>-242</v>
+        <f>E58</f>
+        <v>-921.4</v>
       </c>
       <c r="K58" s="68">
         <f>E58-(I58*NORMINV(0.975,0,1))</f>
-        <v>-289.4311284258693</v>
+        <v>-1101.9910815355206</v>
       </c>
       <c r="L58" s="68">
         <f>E58+(I58*NORMINV(0.975,0,1))</f>
-        <v>-194.5688715741307</v>
+        <v>-740.80891846447946</v>
       </c>
       <c r="N58" s="68" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="59" spans="2:19">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14">
       <c r="B59" s="68" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C59" s="68" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D59" s="68" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E59" s="68">
-        <v>-921.4</v>
+        <v>-1514</v>
       </c>
       <c r="F59" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G59" s="68">
         <v>5</v>
       </c>
       <c r="H59" s="68">
-        <f t="shared" si="11"/>
-        <v>-921.4</v>
+        <f>E59</f>
+        <v>-1514</v>
       </c>
       <c r="I59" s="68">
         <f>-E59*0.1</f>
-        <v>92.14</v>
+        <v>151.4</v>
       </c>
       <c r="J59" s="106">
-        <f>E59</f>
-        <v>-921.4</v>
+        <f t="shared" si="7"/>
+        <v>-1514</v>
       </c>
       <c r="K59" s="68">
         <f>E59-(I59*NORMINV(0.975,0,1))</f>
-        <v>-1101.9910815355206</v>
+        <v>-1810.7385472593642</v>
       </c>
       <c r="L59" s="68">
         <f>E59+(I59*NORMINV(0.975,0,1))</f>
-        <v>-740.80891846447946</v>
+        <v>-1217.2614527406358</v>
       </c>
       <c r="N59" s="68" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="60" spans="2:19">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14">
       <c r="B60" s="68" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C60" s="68" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D60" s="68" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E60" s="68">
-        <v>-1514</v>
+        <v>1446.8</v>
       </c>
       <c r="F60" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G60" s="68">
         <v>5</v>
       </c>
       <c r="H60" s="68">
         <f>E60</f>
-        <v>-1514</v>
-      </c>
-      <c r="I60" s="68">
-        <f>-E60*0.1</f>
-        <v>151.4</v>
+        <v>1446.8</v>
+      </c>
+      <c r="I60" s="100">
+        <f>H60*0.1</f>
+        <v>144.68</v>
       </c>
       <c r="J60" s="106">
         <f t="shared" si="7"/>
-        <v>-1514</v>
-      </c>
-      <c r="K60" s="68">
+        <v>1446.8</v>
+      </c>
+      <c r="K60" s="101">
         <f>E60-(I60*NORMINV(0.975,0,1))</f>
-        <v>-1810.7385472593642</v>
-      </c>
-      <c r="L60" s="68">
+        <v>1163.2324107167451</v>
+      </c>
+      <c r="L60" s="101">
         <f>E60+(I60*NORMINV(0.975,0,1))</f>
-        <v>-1217.2614527406358</v>
+        <v>1730.3675892832548</v>
       </c>
       <c r="N60" s="68" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="61" spans="2:19">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="61" spans="2:14">
       <c r="B61" s="68" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C61" s="68" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D61" s="68" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E61" s="68">
-        <v>1446.8</v>
+        <v>1676.1</v>
       </c>
       <c r="F61" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G61" s="68">
         <v>5</v>
       </c>
       <c r="H61" s="68">
-        <f>E61</f>
-        <v>1446.8</v>
+        <f t="shared" ref="H61:H64" si="12">E61</f>
+        <v>1676.1</v>
       </c>
       <c r="I61" s="100">
         <f>H61*0.1</f>
-        <v>144.68</v>
+        <v>167.61</v>
       </c>
       <c r="J61" s="106">
         <f t="shared" si="7"/>
-        <v>1446.8</v>
+        <v>1676.1</v>
       </c>
       <c r="K61" s="101">
-        <f>E61-(I61*NORMINV(0.975,0,1))</f>
-        <v>1163.2324107167451</v>
+        <f t="shared" ref="K61:K64" si="13">E61-(I61*NORMINV(0.975,0,1))</f>
+        <v>1347.5904365512415</v>
       </c>
       <c r="L61" s="101">
-        <f>E61+(I61*NORMINV(0.975,0,1))</f>
-        <v>1730.3675892832548</v>
+        <f t="shared" ref="L61:L64" si="14">E61+(I61*NORMINV(0.975,0,1))</f>
+        <v>2004.6095634487583</v>
       </c>
       <c r="N61" s="68" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="62" spans="2:19">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14">
       <c r="B62" s="68" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C62" s="68" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D62" s="68" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E62" s="68">
-        <v>1676.1</v>
+        <v>3956.7</v>
       </c>
       <c r="F62" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G62" s="68">
         <v>5</v>
       </c>
       <c r="H62" s="68">
-        <f t="shared" ref="H62:H65" si="12">E62</f>
-        <v>1676.1</v>
+        <f t="shared" si="12"/>
+        <v>3956.7</v>
       </c>
       <c r="I62" s="100">
-        <f>H62*0.1</f>
-        <v>167.61</v>
+        <f t="shared" ref="I62:I64" si="15">H62*0.1</f>
+        <v>395.67</v>
       </c>
       <c r="J62" s="106">
         <f t="shared" si="7"/>
-        <v>1676.1</v>
+        <v>3956.7</v>
       </c>
       <c r="K62" s="101">
-        <f t="shared" ref="K62:K65" si="13">E62-(I62*NORMINV(0.975,0,1))</f>
-        <v>1347.5904365512415</v>
+        <f t="shared" si="13"/>
+        <v>3181.2010502370367</v>
       </c>
       <c r="L62" s="101">
-        <f t="shared" ref="L62:L65" si="14">E62+(I62*NORMINV(0.975,0,1))</f>
-        <v>2004.6095634487583</v>
+        <f t="shared" si="14"/>
+        <v>4732.1989497629629</v>
       </c>
       <c r="N62" s="68" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="63" spans="2:19">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14">
       <c r="B63" s="68" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C63" s="68" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D63" s="68" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E63" s="68">
-        <v>3956.7</v>
+        <v>5406.9</v>
       </c>
       <c r="F63" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G63" s="68">
         <v>5</v>
       </c>
       <c r="H63" s="68">
         <f t="shared" si="12"/>
-        <v>3956.7</v>
+        <v>5406.9</v>
       </c>
       <c r="I63" s="100">
-        <f t="shared" ref="I63:I65" si="15">H63*0.1</f>
-        <v>395.67</v>
+        <f t="shared" si="15"/>
+        <v>540.68999999999994</v>
       </c>
       <c r="J63" s="106">
         <f t="shared" si="7"/>
-        <v>3956.7</v>
+        <v>5406.9</v>
       </c>
       <c r="K63" s="101">
         <f t="shared" si="13"/>
-        <v>3181.2010502370367</v>
+        <v>4347.167073199038</v>
       </c>
       <c r="L63" s="101">
         <f t="shared" si="14"/>
-        <v>4732.1989497629629</v>
+        <v>6466.6329268009613</v>
       </c>
       <c r="N63" s="68" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="64" spans="2:19">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14">
       <c r="B64" s="68" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C64" s="68" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D64" s="68" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E64" s="68">
-        <v>5406.9</v>
+        <v>1217.4000000000001</v>
       </c>
       <c r="F64" s="68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G64" s="68">
         <v>5</v>
       </c>
       <c r="H64" s="68">
         <f t="shared" si="12"/>
-        <v>5406.9</v>
+        <v>1217.4000000000001</v>
       </c>
       <c r="I64" s="100">
         <f t="shared" si="15"/>
-        <v>540.68999999999994</v>
+        <v>121.74000000000001</v>
       </c>
       <c r="J64" s="106">
         <f t="shared" si="7"/>
-        <v>5406.9</v>
+        <v>1217.4000000000001</v>
       </c>
       <c r="K64" s="101">
         <f t="shared" si="13"/>
-        <v>4347.167073199038</v>
+        <v>978.79398452209398</v>
       </c>
       <c r="L64" s="101">
         <f t="shared" si="14"/>
-        <v>6466.6329268009613</v>
+        <v>1456.0060154779062</v>
       </c>
       <c r="N64" s="68" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="65" spans="2:14">
       <c r="B65" s="68" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C65" s="68" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D65" s="68" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="E65" s="68">
-        <v>1217.4000000000001</v>
+        <v>401</v>
       </c>
       <c r="F65" s="68" t="s">
-        <v>254</v>
+        <v>47</v>
       </c>
       <c r="G65" s="68">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H65" s="68">
-        <f t="shared" si="12"/>
-        <v>1217.4000000000001</v>
+        <v>100</v>
       </c>
       <c r="I65" s="100">
-        <f t="shared" si="15"/>
-        <v>121.74000000000001</v>
+        <f>E65/H65</f>
+        <v>4.01</v>
       </c>
       <c r="J65" s="106">
         <f t="shared" si="7"/>
-        <v>1217.4000000000001</v>
+        <v>401</v>
       </c>
       <c r="K65" s="101">
-        <f t="shared" si="13"/>
-        <v>978.79398452209398</v>
+        <f>_xlfn.GAMMA.INV(0.025,H65,I65)</f>
+        <v>326.26960491620173</v>
       </c>
       <c r="L65" s="101">
-        <f t="shared" si="14"/>
-        <v>1456.0060154779062</v>
+        <f>_xlfn.GAMMA.INV(0.975,H65,I65)</f>
+        <v>483.32108049015335</v>
       </c>
       <c r="N65" s="68" t="s">
-        <v>285</v>
+        <v>311</v>
       </c>
     </row>
     <row r="66" spans="2:14">
       <c r="B66" s="68" t="s">
-        <v>288</v>
+        <v>312</v>
       </c>
       <c r="C66" s="68" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D66" s="68" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E66" s="68">
-        <v>401</v>
+        <v>8.57</v>
       </c>
       <c r="F66" s="68" t="s">
         <v>47</v>
@@ -6434,38 +6421,38 @@
       <c r="H66" s="68">
         <v>100</v>
       </c>
-      <c r="I66" s="100">
+      <c r="I66" s="68">
         <f>E66/H66</f>
-        <v>4.01</v>
+        <v>8.5699999999999998E-2</v>
       </c>
       <c r="J66" s="106">
         <f t="shared" si="7"/>
-        <v>401</v>
+        <v>8.57</v>
       </c>
       <c r="K66" s="101">
-        <f>_xlfn.GAMMA.INV(0.025,H66,I66)</f>
-        <v>326.26960491620173</v>
+        <f t="shared" ref="K66:K69" si="16">_xlfn.GAMMA.INV(0.025,H66,I66)</f>
+        <v>6.9728940502041121</v>
       </c>
       <c r="L66" s="101">
-        <f>_xlfn.GAMMA.INV(0.975,H66,I66)</f>
-        <v>483.32108049015335</v>
+        <f t="shared" ref="L66:L69" si="17">_xlfn.GAMMA.INV(0.975,H66,I66)</f>
+        <v>10.329330822445423</v>
       </c>
       <c r="N66" s="68" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="67" spans="2:14">
       <c r="B67" s="68" t="s">
+        <v>312</v>
+      </c>
+      <c r="C67" s="68" t="s">
+        <v>315</v>
+      </c>
+      <c r="D67" s="68" t="s">
         <v>316</v>
       </c>
-      <c r="C67" s="68" t="s">
-        <v>317</v>
-      </c>
-      <c r="D67" s="68" t="s">
-        <v>325</v>
-      </c>
       <c r="E67" s="68">
-        <v>8.57</v>
+        <v>1.3</v>
       </c>
       <c r="F67" s="68" t="s">
         <v>47</v>
@@ -6478,36 +6465,36 @@
       </c>
       <c r="I67" s="68">
         <f>E67/H67</f>
-        <v>8.5699999999999998E-2</v>
+        <v>1.3000000000000001E-2</v>
       </c>
       <c r="J67" s="106">
         <f t="shared" si="7"/>
-        <v>8.57</v>
+        <v>1.3</v>
       </c>
       <c r="K67" s="101">
-        <f t="shared" ref="K67:K70" si="16">_xlfn.GAMMA.INV(0.025,H67,I67)</f>
-        <v>6.9728940502041121</v>
+        <f t="shared" si="16"/>
+        <v>1.0577318862620009</v>
       </c>
       <c r="L67" s="101">
-        <f t="shared" ref="L67:L70" si="17">_xlfn.GAMMA.INV(0.975,H67,I67)</f>
-        <v>10.329330822445423</v>
+        <f t="shared" si="17"/>
+        <v>1.566876320791021</v>
       </c>
       <c r="N67" s="68" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="68" spans="2:14">
       <c r="B68" s="68" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C68" s="68" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D68" s="68" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E68" s="68">
-        <v>1.3</v>
+        <v>11.8</v>
       </c>
       <c r="F68" s="68" t="s">
         <v>47</v>
@@ -6519,37 +6506,37 @@
         <v>100</v>
       </c>
       <c r="I68" s="68">
-        <f>E68/H68</f>
-        <v>1.3000000000000001E-2</v>
+        <f t="shared" ref="I68:I69" si="18">E68/H68</f>
+        <v>0.11800000000000001</v>
       </c>
       <c r="J68" s="106">
         <f t="shared" si="7"/>
-        <v>1.3</v>
+        <v>11.8</v>
       </c>
       <c r="K68" s="101">
         <f t="shared" si="16"/>
-        <v>1.0577318862620009</v>
+        <v>9.6009509676089309</v>
       </c>
       <c r="L68" s="101">
         <f t="shared" si="17"/>
-        <v>1.566876320791021</v>
+        <v>14.222415834872344</v>
       </c>
       <c r="N68" s="68" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="69" spans="2:14">
       <c r="B69" s="68" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C69" s="68" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D69" s="68" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E69" s="68">
-        <v>11.8</v>
+        <v>3.86</v>
       </c>
       <c r="F69" s="68" t="s">
         <v>47</v>
@@ -6561,65 +6548,23 @@
         <v>100</v>
       </c>
       <c r="I69" s="68">
-        <f t="shared" ref="I69:I70" si="18">E69/H69</f>
-        <v>0.11800000000000001</v>
+        <f t="shared" si="18"/>
+        <v>3.8599999999999995E-2</v>
       </c>
       <c r="J69" s="106">
         <f t="shared" si="7"/>
-        <v>11.8</v>
+        <v>3.86</v>
       </c>
       <c r="K69" s="101">
         <f t="shared" si="16"/>
-        <v>9.6009509676089309</v>
+        <v>3.1406500622856326</v>
       </c>
       <c r="L69" s="101">
         <f t="shared" si="17"/>
-        <v>14.222415834872344</v>
+        <v>4.6524173832717999</v>
       </c>
       <c r="N69" s="68" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="70" spans="2:14">
-      <c r="B70" s="68" t="s">
-        <v>316</v>
-      </c>
-      <c r="C70" s="68" t="s">
-        <v>323</v>
-      </c>
-      <c r="D70" s="68" t="s">
-        <v>324</v>
-      </c>
-      <c r="E70" s="68">
-        <v>3.86</v>
-      </c>
-      <c r="F70" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="G70" s="68">
-        <v>2</v>
-      </c>
-      <c r="H70" s="68">
-        <v>100</v>
-      </c>
-      <c r="I70" s="68">
-        <f t="shared" si="18"/>
-        <v>3.8599999999999995E-2</v>
-      </c>
-      <c r="J70" s="106">
-        <f t="shared" si="7"/>
-        <v>3.86</v>
-      </c>
-      <c r="K70" s="101">
-        <f t="shared" si="16"/>
-        <v>3.1406500622856326</v>
-      </c>
-      <c r="L70" s="101">
-        <f t="shared" si="17"/>
-        <v>4.6524173832717999</v>
-      </c>
-      <c r="N70" s="68" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -6641,7 +6586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F32D2E0-32A8-4C75-8C98-9C12E5C1268D}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -6672,7 +6617,7 @@
         <v>40</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -7822,7 +7767,7 @@
     <row r="46" spans="1:6">
       <c r="A46" s="5" t="str">
         <f>parameters!D46</f>
-        <v>Spec.cystoscopy.HG</v>
+        <v>Spec.cystoscopy</v>
       </c>
       <c r="B46" s="113">
         <f>parameters!E46</f>
@@ -7872,600 +7817,600 @@
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="5" t="str">
-        <f>parameters!D48</f>
-        <v>Spec.cystoscopy.LG</v>
-      </c>
-      <c r="B48" s="113">
-        <f>parameters!E48</f>
-        <v>0.76800000000000002</v>
-      </c>
-      <c r="C48" s="112">
-        <f>parameters!G48</f>
-        <v>1</v>
-      </c>
-      <c r="D48" s="114">
-        <f>parameters!H48</f>
-        <v>719</v>
-      </c>
-      <c r="E48" s="114">
-        <f>parameters!I48</f>
-        <v>166.80799999999999</v>
-      </c>
-      <c r="F48" s="114">
-        <f>parameters!J48</f>
-        <v>0.76800000000000002</v>
+      <c r="A48" s="5" t="e">
+        <f>parameters!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B48" s="113" t="e">
+        <f>parameters!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C48" s="112" t="e">
+        <f>parameters!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D48" s="114" t="e">
+        <f>parameters!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E48" s="114" t="e">
+        <f>parameters!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F48" s="114" t="e">
+        <f>parameters!#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="5" t="str">
+        <f>parameters!D48</f>
+        <v>Mort.TURBT</v>
+      </c>
+      <c r="B49" s="113">
+        <f>parameters!E48</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C49" s="112">
+        <f>parameters!G48</f>
+        <v>5</v>
+      </c>
+      <c r="D49" s="114">
+        <f>parameters!H48</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E49" s="114">
+        <f>parameters!I48</f>
+        <v>2.55106728462327E-3</v>
+      </c>
+      <c r="F49" s="114">
+        <f>parameters!J48</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="5" t="str">
         <f>parameters!D49</f>
-        <v>Mort.TURBT</v>
-      </c>
-      <c r="B49" s="113">
+        <v>Utility.age</v>
+      </c>
+      <c r="B50" s="113">
         <f>parameters!E49</f>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="C49" s="112">
+        <v>4.3200000000000001E-3</v>
+      </c>
+      <c r="C50" s="112">
         <f>parameters!G49</f>
         <v>5</v>
       </c>
-      <c r="D49" s="114">
+      <c r="D50" s="114">
         <f>parameters!H49</f>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="E49" s="114">
+        <v>4.3200000000000001E-3</v>
+      </c>
+      <c r="E50" s="114">
         <f>parameters!I49</f>
-        <v>2.55106728462327E-3</v>
-      </c>
-      <c r="F49" s="114">
+        <v>1.4285976793890307E-4</v>
+      </c>
+      <c r="F50" s="114">
         <f>parameters!J49</f>
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="5" t="str">
+        <v>4.3200000000000001E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="5" t="str">
         <f>parameters!D50</f>
-        <v>Utility.age</v>
-      </c>
-      <c r="B50" s="113">
+        <v>Disutility.HG.St1.3</v>
+      </c>
+      <c r="B51" s="113">
         <f>parameters!E50</f>
-        <v>4.3200000000000001E-3</v>
-      </c>
-      <c r="C50" s="112">
+        <v>-0.08</v>
+      </c>
+      <c r="C51" s="112">
         <f>parameters!G50</f>
         <v>5</v>
       </c>
-      <c r="D50" s="114">
+      <c r="D51" s="114">
         <f>parameters!H50</f>
-        <v>4.3200000000000001E-3</v>
-      </c>
-      <c r="E50" s="114">
+        <v>-0.08</v>
+      </c>
+      <c r="E51" s="114">
         <f>parameters!I50</f>
-        <v>1.4285976793890307E-4</v>
-      </c>
-      <c r="F50" s="114">
+        <v>4.3368143838595594E-2</v>
+      </c>
+      <c r="F51" s="114">
         <f>parameters!J50</f>
-        <v>4.3200000000000001E-3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="5" t="str">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="5" t="str">
         <f>parameters!D51</f>
-        <v>Disutility.HG.St1.3</v>
-      </c>
-      <c r="B51" s="113">
+        <v>Disutility.HG.St4</v>
+      </c>
+      <c r="B52" s="113">
         <f>parameters!E51</f>
-        <v>-0.08</v>
-      </c>
-      <c r="C51" s="112">
+        <v>-0.18</v>
+      </c>
+      <c r="C52" s="112">
         <f>parameters!G51</f>
         <v>5</v>
       </c>
-      <c r="D51" s="114">
+      <c r="D52" s="114">
         <f>parameters!H51</f>
-        <v>-0.08</v>
-      </c>
-      <c r="E51" s="114">
+        <v>-0.18</v>
+      </c>
+      <c r="E52" s="114">
         <f>parameters!I51</f>
-        <v>4.3368143838595594E-2</v>
-      </c>
-      <c r="F51" s="114">
+        <v>6.1225614830958487E-2</v>
+      </c>
+      <c r="F52" s="114">
         <f>parameters!J51</f>
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="5" t="str">
-        <f>parameters!D52</f>
-        <v>Disutility.HG.St4</v>
-      </c>
-      <c r="B52" s="113">
-        <f>parameters!E52</f>
-        <v>-0.18</v>
-      </c>
-      <c r="C52" s="112">
-        <f>parameters!G52</f>
-        <v>5</v>
-      </c>
-      <c r="D52" s="114">
-        <f>parameters!H52</f>
-        <v>-0.18</v>
-      </c>
-      <c r="E52" s="114">
-        <f>parameters!I52</f>
-        <v>6.1225614830958487E-2</v>
-      </c>
-      <c r="F52" s="114">
-        <f>parameters!J52</f>
         <v>-0.18</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="5" t="str">
-        <f>parameters!D53</f>
+        <f>parameters!D52</f>
         <v>Disutility.LG</v>
       </c>
       <c r="B53" s="113">
-        <f>parameters!E53</f>
+        <f>parameters!E52</f>
         <v>0</v>
       </c>
       <c r="C53" s="112">
-        <f>parameters!G53</f>
+        <f>parameters!G52</f>
         <v>6</v>
       </c>
       <c r="D53" s="114">
-        <f>parameters!H53</f>
+        <f>parameters!H52</f>
         <v>0</v>
       </c>
       <c r="E53" s="114">
-        <f>parameters!I53</f>
+        <f>parameters!I52</f>
         <v>0</v>
       </c>
       <c r="F53" s="114">
-        <f>parameters!J53</f>
+        <f>parameters!J52</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="5" t="str">
+        <f>parameters!D53</f>
+        <v>Cost.diag.sympt</v>
+      </c>
+      <c r="B54" s="113">
+        <f>parameters!E53</f>
+        <v>610.58000000000004</v>
+      </c>
+      <c r="C54" s="112">
+        <f>parameters!G53</f>
+        <v>2</v>
+      </c>
+      <c r="D54" s="114">
+        <f>parameters!H53</f>
+        <v>100</v>
+      </c>
+      <c r="E54" s="114">
+        <f>parameters!I53</f>
+        <v>6.1058000000000003</v>
+      </c>
+      <c r="F54" s="114">
+        <f>parameters!J53</f>
+        <v>610.58000000000004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="5" t="str">
         <f>parameters!D54</f>
-        <v>Cost.diag.sympt</v>
-      </c>
-      <c r="B54" s="113">
+        <v>Cost.diag.screen</v>
+      </c>
+      <c r="B55" s="113">
         <f>parameters!E54</f>
-        <v>610.58000000000004</v>
-      </c>
-      <c r="C54" s="112">
+        <v>584.89</v>
+      </c>
+      <c r="C55" s="112">
         <f>parameters!G54</f>
         <v>2</v>
       </c>
-      <c r="D54" s="114">
+      <c r="D55" s="114">
         <f>parameters!H54</f>
         <v>100</v>
       </c>
-      <c r="E54" s="114">
+      <c r="E55" s="114">
         <f>parameters!I54</f>
-        <v>6.1058000000000003</v>
-      </c>
-      <c r="F54" s="114">
+        <v>5.8488999999999995</v>
+      </c>
+      <c r="F55" s="114">
         <f>parameters!J54</f>
-        <v>610.58000000000004</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="5" t="str">
+        <v>584.89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="5" t="str">
         <f>parameters!D55</f>
-        <v>Cost.diag.screen</v>
-      </c>
-      <c r="B55" s="113">
+        <v>Cost.treat.intercept</v>
+      </c>
+      <c r="B56" s="113">
         <f>parameters!E55</f>
-        <v>584.89</v>
-      </c>
-      <c r="C55" s="112">
+        <v>2348.8000000000002</v>
+      </c>
+      <c r="C56" s="112">
         <f>parameters!G55</f>
         <v>2</v>
       </c>
-      <c r="D55" s="114">
+      <c r="D56" s="114">
         <f>parameters!H55</f>
         <v>100</v>
       </c>
-      <c r="E55" s="114">
+      <c r="E56" s="114">
         <f>parameters!I55</f>
-        <v>5.8488999999999995</v>
-      </c>
-      <c r="F55" s="114">
+        <v>23.488000000000003</v>
+      </c>
+      <c r="F56" s="114">
         <f>parameters!J55</f>
-        <v>584.89</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="5" t="str">
-        <f>parameters!D56</f>
-        <v>Cost.treat.intercept</v>
-      </c>
-      <c r="B56" s="113">
-        <f>parameters!E56</f>
-        <v>2348.8000000000002</v>
-      </c>
-      <c r="C56" s="112">
-        <f>parameters!G56</f>
-        <v>2</v>
-      </c>
-      <c r="D56" s="114">
-        <f>parameters!H56</f>
-        <v>100</v>
-      </c>
-      <c r="E56" s="114">
-        <f>parameters!I56</f>
-        <v>23.488000000000003</v>
-      </c>
-      <c r="F56" s="114">
-        <f>parameters!J56</f>
         <v>2348.8000000000002</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="5" t="str">
+        <f>parameters!D56</f>
+        <v>Cost.treat.past.smoke</v>
+      </c>
+      <c r="B57" s="113">
+        <f>parameters!E56</f>
+        <v>-57.2</v>
+      </c>
+      <c r="C57" s="112">
+        <f>parameters!G56</f>
+        <v>5</v>
+      </c>
+      <c r="D57" s="114">
+        <f>parameters!H56</f>
+        <v>-57.2</v>
+      </c>
+      <c r="E57" s="114">
+        <f>parameters!I56</f>
+        <v>5.7200000000000006</v>
+      </c>
+      <c r="F57" s="114">
+        <f>parameters!J56</f>
+        <v>-57.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="5" t="str">
         <f>parameters!D57</f>
-        <v>Cost.treat.past.smoke</v>
-      </c>
-      <c r="B57" s="113">
+        <v>Cost.treat.current.smoke</v>
+      </c>
+      <c r="B58" s="113">
         <f>parameters!E57</f>
-        <v>-57.2</v>
-      </c>
-      <c r="C57" s="112">
+        <v>-242</v>
+      </c>
+      <c r="C58" s="112">
         <f>parameters!G57</f>
         <v>5</v>
       </c>
-      <c r="D57" s="114">
+      <c r="D58" s="114">
         <f>parameters!H57</f>
-        <v>-57.2</v>
-      </c>
-      <c r="E57" s="114">
+        <v>-242</v>
+      </c>
+      <c r="E58" s="114">
         <f>parameters!I57</f>
-        <v>5.7200000000000006</v>
-      </c>
-      <c r="F57" s="114">
+        <v>24.200000000000003</v>
+      </c>
+      <c r="F58" s="114">
         <f>parameters!J57</f>
-        <v>-57.2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="5" t="str">
+        <v>-242</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="5" t="str">
         <f>parameters!D58</f>
-        <v>Cost.treat.current.smoke</v>
-      </c>
-      <c r="B58" s="113">
+        <v>Cost.treat.Y2</v>
+      </c>
+      <c r="B59" s="113">
         <f>parameters!E58</f>
-        <v>-242</v>
-      </c>
-      <c r="C58" s="112">
+        <v>-921.4</v>
+      </c>
+      <c r="C59" s="112">
         <f>parameters!G58</f>
         <v>5</v>
       </c>
-      <c r="D58" s="114">
+      <c r="D59" s="114">
         <f>parameters!H58</f>
-        <v>-242</v>
-      </c>
-      <c r="E58" s="114">
+        <v>-921.4</v>
+      </c>
+      <c r="E59" s="114">
         <f>parameters!I58</f>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="F58" s="114">
+        <v>92.14</v>
+      </c>
+      <c r="F59" s="114">
         <f>parameters!J58</f>
-        <v>-242</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="5" t="str">
+        <v>-921.4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="5" t="str">
         <f>parameters!D59</f>
-        <v>Cost.treat.Y2</v>
-      </c>
-      <c r="B59" s="113">
+        <v>Cost.treat.Y3</v>
+      </c>
+      <c r="B60" s="113">
         <f>parameters!E59</f>
-        <v>-921.4</v>
-      </c>
-      <c r="C59" s="112">
+        <v>-1514</v>
+      </c>
+      <c r="C60" s="112">
         <f>parameters!G59</f>
         <v>5</v>
       </c>
-      <c r="D59" s="114">
+      <c r="D60" s="114">
         <f>parameters!H59</f>
-        <v>-921.4</v>
-      </c>
-      <c r="E59" s="114">
+        <v>-1514</v>
+      </c>
+      <c r="E60" s="114">
         <f>parameters!I59</f>
-        <v>92.14</v>
-      </c>
-      <c r="F59" s="114">
+        <v>151.4</v>
+      </c>
+      <c r="F60" s="114">
         <f>parameters!J59</f>
-        <v>-921.4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="5" t="str">
+        <v>-1514</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="5" t="str">
         <f>parameters!D60</f>
-        <v>Cost.treat.Y3</v>
-      </c>
-      <c r="B60" s="113">
+        <v>Cost.treat.stage1</v>
+      </c>
+      <c r="B61" s="113">
         <f>parameters!E60</f>
-        <v>-1514</v>
-      </c>
-      <c r="C60" s="112">
+        <v>1446.8</v>
+      </c>
+      <c r="C61" s="112">
         <f>parameters!G60</f>
         <v>5</v>
       </c>
-      <c r="D60" s="114">
+      <c r="D61" s="114">
         <f>parameters!H60</f>
-        <v>-1514</v>
-      </c>
-      <c r="E60" s="114">
+        <v>1446.8</v>
+      </c>
+      <c r="E61" s="114">
         <f>parameters!I60</f>
-        <v>151.4</v>
-      </c>
-      <c r="F60" s="114">
+        <v>144.68</v>
+      </c>
+      <c r="F61" s="114">
         <f>parameters!J60</f>
-        <v>-1514</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="5" t="str">
+        <v>1446.8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="5" t="str">
         <f>parameters!D61</f>
-        <v>Cost.treat.stage1</v>
-      </c>
-      <c r="B61" s="113">
+        <v>Cost.treat.stage2</v>
+      </c>
+      <c r="B62" s="113">
         <f>parameters!E61</f>
-        <v>1446.8</v>
-      </c>
-      <c r="C61" s="112">
+        <v>1676.1</v>
+      </c>
+      <c r="C62" s="112">
         <f>parameters!G61</f>
         <v>5</v>
       </c>
-      <c r="D61" s="114">
+      <c r="D62" s="114">
         <f>parameters!H61</f>
-        <v>1446.8</v>
-      </c>
-      <c r="E61" s="114">
+        <v>1676.1</v>
+      </c>
+      <c r="E62" s="114">
         <f>parameters!I61</f>
-        <v>144.68</v>
-      </c>
-      <c r="F61" s="114">
+        <v>167.61</v>
+      </c>
+      <c r="F62" s="114">
         <f>parameters!J61</f>
-        <v>1446.8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="5" t="str">
+        <v>1676.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="5" t="str">
         <f>parameters!D62</f>
-        <v>Cost.treat.stage2</v>
-      </c>
-      <c r="B62" s="113">
+        <v>Cost.treat.stage3</v>
+      </c>
+      <c r="B63" s="113">
         <f>parameters!E62</f>
-        <v>1676.1</v>
-      </c>
-      <c r="C62" s="112">
+        <v>3956.7</v>
+      </c>
+      <c r="C63" s="112">
         <f>parameters!G62</f>
         <v>5</v>
       </c>
-      <c r="D62" s="114">
+      <c r="D63" s="114">
         <f>parameters!H62</f>
-        <v>1676.1</v>
-      </c>
-      <c r="E62" s="114">
+        <v>3956.7</v>
+      </c>
+      <c r="E63" s="114">
         <f>parameters!I62</f>
-        <v>167.61</v>
-      </c>
-      <c r="F62" s="114">
+        <v>395.67</v>
+      </c>
+      <c r="F63" s="114">
         <f>parameters!J62</f>
-        <v>1676.1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="5" t="str">
+        <v>3956.7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="5" t="str">
         <f>parameters!D63</f>
-        <v>Cost.treat.stage3</v>
-      </c>
-      <c r="B63" s="113">
+        <v>Cost.treat.stage4</v>
+      </c>
+      <c r="B64" s="113">
         <f>parameters!E63</f>
-        <v>3956.7</v>
-      </c>
-      <c r="C63" s="112">
+        <v>5406.9</v>
+      </c>
+      <c r="C64" s="112">
         <f>parameters!G63</f>
         <v>5</v>
       </c>
-      <c r="D63" s="114">
+      <c r="D64" s="114">
         <f>parameters!H63</f>
-        <v>3956.7</v>
-      </c>
-      <c r="E63" s="114">
+        <v>5406.9</v>
+      </c>
+      <c r="E64" s="114">
         <f>parameters!I63</f>
-        <v>395.67</v>
-      </c>
-      <c r="F63" s="114">
+        <v>540.68999999999994</v>
+      </c>
+      <c r="F64" s="114">
         <f>parameters!J63</f>
-        <v>3956.7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="5" t="str">
+        <v>5406.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="5" t="str">
         <f>parameters!D64</f>
-        <v>Cost.treat.stage4</v>
-      </c>
-      <c r="B64" s="113">
+        <v>Cost.treat.LG</v>
+      </c>
+      <c r="B65" s="113">
         <f>parameters!E64</f>
-        <v>5406.9</v>
-      </c>
-      <c r="C64" s="112">
+        <v>1217.4000000000001</v>
+      </c>
+      <c r="C65" s="112">
         <f>parameters!G64</f>
         <v>5</v>
       </c>
-      <c r="D64" s="114">
+      <c r="D65" s="114">
         <f>parameters!H64</f>
-        <v>5406.9</v>
-      </c>
-      <c r="E64" s="114">
+        <v>1217.4000000000001</v>
+      </c>
+      <c r="E65" s="114">
         <f>parameters!I64</f>
-        <v>540.68999999999994</v>
-      </c>
-      <c r="F64" s="114">
+        <v>121.74000000000001</v>
+      </c>
+      <c r="F65" s="114">
         <f>parameters!J64</f>
-        <v>5406.9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="5" t="str">
-        <f>parameters!D65</f>
-        <v>Cost.treat.LG</v>
-      </c>
-      <c r="B65" s="113">
-        <f>parameters!E65</f>
-        <v>1217.4000000000001</v>
-      </c>
-      <c r="C65" s="112">
-        <f>parameters!G65</f>
-        <v>5</v>
-      </c>
-      <c r="D65" s="114">
-        <f>parameters!H65</f>
-        <v>1217.4000000000001</v>
-      </c>
-      <c r="E65" s="114">
-        <f>parameters!I65</f>
-        <v>121.74000000000001</v>
-      </c>
-      <c r="F65" s="114">
-        <f>parameters!J65</f>
         <v>1217.4000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="5" t="str">
+        <f>parameters!D65</f>
+        <v>Cost.surv.Y4.5</v>
+      </c>
+      <c r="B66" s="113">
+        <f>parameters!E65</f>
+        <v>401</v>
+      </c>
+      <c r="C66" s="112">
+        <f>parameters!G65</f>
+        <v>2</v>
+      </c>
+      <c r="D66" s="114">
+        <f>parameters!H65</f>
+        <v>100</v>
+      </c>
+      <c r="E66" s="114">
+        <f>parameters!I65</f>
+        <v>4.01</v>
+      </c>
+      <c r="F66" s="114">
+        <f>parameters!J65</f>
+        <v>401</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="5" t="str">
         <f>parameters!D66</f>
-        <v>Cost.surv.Y4.5</v>
-      </c>
-      <c r="B66" s="113">
+        <v>Cost.dipstick.invite</v>
+      </c>
+      <c r="B67" s="113">
         <f>parameters!E66</f>
-        <v>401</v>
-      </c>
-      <c r="C66" s="112">
+        <v>8.57</v>
+      </c>
+      <c r="C67" s="112">
         <f>parameters!G66</f>
         <v>2</v>
       </c>
-      <c r="D66" s="114">
+      <c r="D67" s="114">
         <f>parameters!H66</f>
         <v>100</v>
       </c>
-      <c r="E66" s="114">
+      <c r="E67" s="114">
         <f>parameters!I66</f>
-        <v>4.01</v>
-      </c>
-      <c r="F66" s="114">
+        <v>8.5699999999999998E-2</v>
+      </c>
+      <c r="F67" s="114">
         <f>parameters!J66</f>
-        <v>401</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="5" t="str">
+        <v>8.57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="5" t="str">
         <f>parameters!D67</f>
-        <v>Cost.dipstick.invite</v>
-      </c>
-      <c r="B67" s="113">
+        <v>Cost.ad.dipstick</v>
+      </c>
+      <c r="B68" s="113">
         <f>parameters!E67</f>
-        <v>8.57</v>
-      </c>
-      <c r="C67" s="112">
+        <v>1.3</v>
+      </c>
+      <c r="C68" s="112">
         <f>parameters!G67</f>
         <v>2</v>
       </c>
-      <c r="D67" s="114">
+      <c r="D68" s="114">
         <f>parameters!H67</f>
         <v>100</v>
       </c>
-      <c r="E67" s="114">
+      <c r="E68" s="114">
         <f>parameters!I67</f>
-        <v>8.5699999999999998E-2</v>
-      </c>
-      <c r="F67" s="114">
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="F68" s="114">
         <f>parameters!J67</f>
-        <v>8.57</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="5" t="str">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="5" t="str">
         <f>parameters!D68</f>
-        <v>Cost.ad.dipstick</v>
-      </c>
-      <c r="B68" s="113">
+        <v>Cost.dipstick.positive</v>
+      </c>
+      <c r="B69" s="113">
         <f>parameters!E68</f>
-        <v>1.3</v>
-      </c>
-      <c r="C68" s="112">
+        <v>11.8</v>
+      </c>
+      <c r="C69" s="112">
         <f>parameters!G68</f>
         <v>2</v>
       </c>
-      <c r="D68" s="114">
+      <c r="D69" s="114">
         <f>parameters!H68</f>
         <v>100</v>
       </c>
-      <c r="E68" s="114">
+      <c r="E69" s="114">
         <f>parameters!I68</f>
-        <v>1.3000000000000001E-2</v>
-      </c>
-      <c r="F68" s="114">
+        <v>0.11800000000000001</v>
+      </c>
+      <c r="F69" s="114">
         <f>parameters!J68</f>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="5" t="str">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="5" t="str">
         <f>parameters!D69</f>
-        <v>Cost.dipstick.positive</v>
-      </c>
-      <c r="B69" s="113">
+        <v>Cost.dipstick</v>
+      </c>
+      <c r="B70" s="113">
         <f>parameters!E69</f>
-        <v>11.8</v>
-      </c>
-      <c r="C69" s="112">
+        <v>3.86</v>
+      </c>
+      <c r="C70" s="112">
         <f>parameters!G69</f>
         <v>2</v>
       </c>
-      <c r="D69" s="114">
+      <c r="D70" s="114">
         <f>parameters!H69</f>
         <v>100</v>
       </c>
-      <c r="E69" s="114">
+      <c r="E70" s="114">
         <f>parameters!I69</f>
-        <v>0.11800000000000001</v>
-      </c>
-      <c r="F69" s="114">
+        <v>3.8599999999999995E-2</v>
+      </c>
+      <c r="F70" s="114">
         <f>parameters!J69</f>
-        <v>11.8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="5" t="str">
-        <f>parameters!D70</f>
-        <v>Cost.dipstick</v>
-      </c>
-      <c r="B70" s="113">
-        <f>parameters!E70</f>
-        <v>3.86</v>
-      </c>
-      <c r="C70" s="112">
-        <f>parameters!G70</f>
-        <v>2</v>
-      </c>
-      <c r="D70" s="114">
-        <f>parameters!H70</f>
-        <v>100</v>
-      </c>
-      <c r="E70" s="114">
-        <f>parameters!I70</f>
-        <v>3.8599999999999995E-2</v>
-      </c>
-      <c r="F70" s="114">
-        <f>parameters!J70</f>
         <v>3.86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing error in non-cohort runs
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cm1om\Documents\Research\Cancer\Bladder\Bladder_cancer_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCCF5E9-C399-4F55-B0CF-2FA221CF9B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8F6227-CB3C-4D53-9C39-D4FD669D3FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1AD6D928-CCB7-482A-A47C-26785A7D3A52}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1AD6D928-CCB7-482A-A47C-26785A7D3A52}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,10 @@
     <sheet name="BCsurv_original" sheetId="6" r:id="rId6"/>
     <sheet name="mortality" sheetId="7" r:id="rId7"/>
     <sheet name="Survival" sheetId="8" r:id="rId8"/>
+    <sheet name="sensitivity" sheetId="9" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="All_cause_mort">OC_mortality_details!$T$26:$AN$28</definedName>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3209" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3250" uniqueCount="373">
   <si>
     <t>Param number</t>
   </si>
@@ -1207,12 +1208,6 @@
     <t xml:space="preserve">the National tariffs / NHS reference costs (2022/23);Lyratzopoulos (2013) </t>
   </si>
   <si>
-    <t>Average diagnostic costs for screen-detected cases</t>
-  </si>
-  <si>
-    <t>Cost.diag.screen</t>
-  </si>
-  <si>
     <t>Costs for treatment and surveillance: intercept (Regression)</t>
   </si>
   <si>
@@ -1379,6 +1374,102 @@
   </si>
   <si>
     <t xml:space="preserve"> study from England Blick (2012  ) [0.94 (95% CI 0.92–0.96)]; scenario: Meta-analysis Zheng (2012); </t>
+  </si>
+  <si>
+    <t>Houguang He</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3892/ol.2016.4556</t>
+  </si>
+  <si>
+    <t>urine cytology test</t>
+  </si>
+  <si>
+    <t>sensitivity</t>
+  </si>
+  <si>
+    <t>specificity</t>
+  </si>
+  <si>
+    <t>cI</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ejrad.2010.04.003</t>
+  </si>
+  <si>
+    <t>ultrasonography for bladder cancer detection:</t>
+  </si>
+  <si>
+    <t>Xinhua Qu</t>
+  </si>
+  <si>
+    <t>joined sensitivity</t>
+  </si>
+  <si>
+    <t>Joined specificity of US+cytology</t>
+  </si>
+  <si>
+    <t>Spec.joined.diag</t>
+  </si>
+  <si>
+    <t>Average diagnostic costs for screen-detected cases, 1st stage in GP center</t>
+  </si>
+  <si>
+    <t>Cost.diag.screen1</t>
+  </si>
+  <si>
+    <t>Cost.diag.screen2</t>
+  </si>
+  <si>
+    <t>Average diagnostic costs for screen-detected cases, 2st stage in haematuria center</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.urolonc.2014.06.008</t>
+  </si>
+  <si>
+    <t>cytology low grade</t>
+  </si>
+  <si>
+    <t>cytology high grade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faysal A. Yafi </t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>relative to total</t>
+  </si>
+  <si>
+    <t>joined sensitivity low risk</t>
+  </si>
+  <si>
+    <t>joined sensitivity high risk</t>
+  </si>
+  <si>
+    <t>Joined sensitivity of US+cytology (HG)</t>
+  </si>
+  <si>
+    <t>Joined sensitivity of US+cytology (LG)</t>
+  </si>
+  <si>
+    <t>Sens.joined.diag.HG</t>
+  </si>
+  <si>
+    <t>Sens.joined.diag.LG</t>
+  </si>
+  <si>
+    <t>combination of data from 2 meta-analyses and a study reporting the sens by grade (see sensitivity page)</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s10549-018-4877-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difference in survival in screen detected vs symptomatic cancers </t>
   </si>
 </sst>
 </file>
@@ -1888,7 +1979,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2116,6 +2207,11 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3497,10 +3593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8694223C-410D-4023-9128-3FD5F8A481E4}">
-  <dimension ref="A1:Z69"/>
+  <dimension ref="A1:Z74"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="N47" sqref="N47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3545,17 +3641,17 @@
       <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="116" t="s">
+      <c r="H1" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="116"/>
+      <c r="I1" s="121"/>
       <c r="J1" s="105" t="s">
-        <v>325</v>
-      </c>
-      <c r="K1" s="117" t="s">
+        <v>323</v>
+      </c>
+      <c r="K1" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="117"/>
+      <c r="L1" s="122"/>
       <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
@@ -3587,7 +3683,7 @@
         <v>9.8400000000000007E-6</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G2" s="5">
         <v>7</v>
@@ -3605,7 +3701,7 @@
         <v>0.01</v>
       </c>
       <c r="N2" s="68" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="O2" s="95"/>
       <c r="P2" s="68">
@@ -3650,7 +3746,7 @@
         <v>0.65200000000000002</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G3" s="5">
         <v>7</v>
@@ -3668,7 +3764,7 @@
         <v>0.05</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="O3" s="96" t="s">
         <v>36</v>
@@ -3995,7 +4091,7 @@
         <v>1.67E-2</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G9" s="5">
         <v>7</v>
@@ -4125,7 +4221,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G12" s="5">
         <v>7</v>
@@ -4154,17 +4250,17 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D13" s="68" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E13" s="110">
         <f>H13</f>
         <v>0.121</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G13" s="5">
         <v>7</v>
@@ -4190,17 +4286,17 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D14" s="68" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E14" s="110">
         <f t="shared" ref="E14:E15" si="2">H14</f>
         <v>0.22700000000000001</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G14" s="5">
         <v>7</v>
@@ -4227,10 +4323,10 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D15" s="68" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E15" s="110">
         <f t="shared" si="2"/>
@@ -4273,7 +4369,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G16" s="5">
         <v>4</v>
@@ -4465,7 +4561,7 @@
         <v>0.66200000000000003</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G21" s="5">
         <v>7</v>
@@ -4503,7 +4599,7 @@
         <v>0.76600000000000001</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G22" s="5">
         <v>7</v>
@@ -4540,7 +4636,7 @@
         <v>0.42299999999999999</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G23" s="5">
         <v>7</v>
@@ -4567,7 +4663,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>78</v>
@@ -4577,7 +4673,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G24" s="5">
         <v>7</v>
@@ -4661,10 +4757,10 @@
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D26" s="106" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E26" s="111">
         <f>H26</f>
@@ -4716,7 +4812,7 @@
         <v>4.4760529439603229E-2</v>
       </c>
       <c r="J27" s="106">
-        <f t="shared" ref="J27:J69" si="7">E27</f>
+        <f t="shared" ref="J27:J74" si="7">E27</f>
         <v>0.70957585397710221</v>
       </c>
       <c r="K27" s="68">
@@ -4980,16 +5076,16 @@
         <v>218</v>
       </c>
       <c r="C34" s="104" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D34" s="104" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E34" s="104">
         <v>1.8794650496471605</v>
       </c>
       <c r="F34" s="104" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G34" s="104">
         <v>5</v>
@@ -4998,10 +5094,10 @@
         <v>1.8794650496471605</v>
       </c>
       <c r="I34" s="104">
-        <v>3.5350227786655028E-3</v>
+        <v>3.5350227786655002E-3</v>
       </c>
       <c r="J34" s="106">
-        <f t="shared" si="7"/>
+        <f>E34</f>
         <v>1.8794650496471605</v>
       </c>
       <c r="K34" s="104">
@@ -5044,7 +5140,7 @@
         <v>8.2744570841605074E-3</v>
       </c>
       <c r="J35" s="106">
-        <f t="shared" si="7"/>
+        <f>E35</f>
         <v>-7.2570692834835374E-2</v>
       </c>
       <c r="K35" s="68">
@@ -5417,7 +5513,7 @@
         <v>0.93</v>
       </c>
       <c r="N44" s="109" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="Q44" s="31" t="s">
         <v>247</v>
@@ -5461,7 +5557,7 @@
         <v>0.98915586560636681</v>
       </c>
       <c r="N45" s="97" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="Q45" s="92" t="s">
         <v>243</v>
@@ -5474,10 +5570,10 @@
         <v>236</v>
       </c>
       <c r="C46" s="99" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D46" s="68" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E46" s="97">
         <v>0.94</v>
@@ -5508,7 +5604,7 @@
         <v>0.9586880948079739</v>
       </c>
       <c r="N46" s="97" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="Q46" s="92" t="s">
         <v>244</v>
@@ -5554,7 +5650,7 @@
         <v>0.98915586560636681</v>
       </c>
       <c r="N47" s="97" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="Q47" s="92">
         <v>0.878</v>
@@ -5564,726 +5660,734 @@
       </c>
       <c r="S47" s="92"/>
     </row>
-    <row r="48" spans="2:19">
-      <c r="B48" s="68" t="s">
-        <v>270</v>
-      </c>
-      <c r="C48" s="68" t="s">
-        <v>79</v>
-      </c>
-      <c r="D48" s="68" t="s">
-        <v>271</v>
-      </c>
-      <c r="E48" s="68">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="F48" s="68" t="s">
+    <row r="48" spans="2:19" s="116" customFormat="1">
+      <c r="B48" s="116" t="s">
+        <v>236</v>
+      </c>
+      <c r="C48" s="99" t="s">
+        <v>366</v>
+      </c>
+      <c r="D48" s="116" t="s">
+        <v>368</v>
+      </c>
+      <c r="E48" s="97">
+        <f>H48</f>
+        <v>0.77159949999999999</v>
+      </c>
+      <c r="F48" s="116" t="s">
         <v>249</v>
       </c>
-      <c r="G48" s="68">
+      <c r="G48" s="116">
         <v>5</v>
       </c>
-      <c r="H48" s="68">
-        <f>E48</f>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="I48" s="100">
+      <c r="H48" s="116">
+        <f>sensitivity!D11</f>
+        <v>0.77159949999999999</v>
+      </c>
+      <c r="I48" s="116">
         <f>(L48-K48)/(2*NORMINV(0.975,0,1))</f>
-        <v>2.55106728462327E-3</v>
-      </c>
-      <c r="J48" s="106">
-        <f t="shared" si="7"/>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="K48" s="101">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="L48" s="101">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="N48" s="68" t="s">
-        <v>272</v>
-      </c>
-      <c r="O48" s="68" t="s">
-        <v>80</v>
+        <v>4.8441961560982842E-2</v>
+      </c>
+      <c r="J48" s="116">
+        <f>H48</f>
+        <v>0.77159949999999999</v>
+      </c>
+      <c r="K48" s="92">
+        <f>sensitivity!E11</f>
+        <v>0.678342</v>
+      </c>
+      <c r="L48" s="92">
+        <f>sensitivity!F11</f>
+        <v>0.86823100000000009</v>
+      </c>
+      <c r="N48" s="97" t="s">
+        <v>370</v>
       </c>
       <c r="Q48" s="92"/>
       <c r="R48" s="92"/>
       <c r="S48" s="92"/>
     </row>
-    <row r="49" spans="2:14">
-      <c r="B49" s="68" t="s">
+    <row r="49" spans="2:19" s="119" customFormat="1">
+      <c r="B49" s="119" t="s">
+        <v>236</v>
+      </c>
+      <c r="C49" s="99" t="s">
+        <v>367</v>
+      </c>
+      <c r="D49" s="119" t="s">
+        <v>369</v>
+      </c>
+      <c r="E49" s="97">
+        <f>H49</f>
+        <v>0.1469713333333334</v>
+      </c>
+      <c r="F49" s="119" t="s">
+        <v>249</v>
+      </c>
+      <c r="G49" s="119">
+        <v>5</v>
+      </c>
+      <c r="H49" s="119">
+        <f>sensitivity!D12</f>
+        <v>0.1469713333333334</v>
+      </c>
+      <c r="I49" s="119">
+        <f>(L49-K49)/(2*NORMINV(0.975,0,1))</f>
+        <v>9.2270402973300605E-3</v>
+      </c>
+      <c r="J49" s="119">
+        <f>H49</f>
+        <v>0.1469713333333334</v>
+      </c>
+      <c r="K49" s="92">
+        <f>sensitivity!E12</f>
+        <v>0.12920800000000005</v>
+      </c>
+      <c r="L49" s="92">
+        <f>sensitivity!F12</f>
+        <v>0.16537733333333338</v>
+      </c>
+      <c r="N49" s="97" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q49" s="92"/>
+      <c r="R49" s="92"/>
+      <c r="S49" s="92"/>
+    </row>
+    <row r="50" spans="2:19" s="116" customFormat="1">
+      <c r="B50" s="116" t="s">
+        <v>236</v>
+      </c>
+      <c r="C50" s="99" t="s">
+        <v>352</v>
+      </c>
+      <c r="D50" s="116" t="s">
+        <v>353</v>
+      </c>
+      <c r="E50" s="97">
+        <f>H50</f>
+        <v>0.99642799999999998</v>
+      </c>
+      <c r="F50" s="116" t="s">
+        <v>249</v>
+      </c>
+      <c r="G50" s="116">
+        <v>5</v>
+      </c>
+      <c r="H50" s="116">
+        <f>sensitivity!G5</f>
+        <v>0.99642799999999998</v>
+      </c>
+      <c r="I50" s="116">
+        <f t="shared" ref="I50:I54" si="8">(L50-K50)/(2*NORMINV(0.975,0,1))</f>
+        <v>7.4593207402382552E-4</v>
+      </c>
+      <c r="J50" s="116">
+        <f>H50</f>
+        <v>0.99642799999999998</v>
+      </c>
+      <c r="K50" s="92">
+        <f>sensitivity!H5</f>
+        <v>0.99468900000000005</v>
+      </c>
+      <c r="L50" s="92">
+        <f>sensitivity!I5</f>
+        <v>0.99761299999999997</v>
+      </c>
+      <c r="N50" s="97" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q50" s="92"/>
+      <c r="R50" s="92"/>
+      <c r="S50" s="92"/>
+    </row>
+    <row r="51" spans="2:19">
+      <c r="B51" s="68" t="s">
+        <v>270</v>
+      </c>
+      <c r="C51" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="68" t="s">
+        <v>271</v>
+      </c>
+      <c r="E51" s="68">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F51" s="68" t="s">
+        <v>249</v>
+      </c>
+      <c r="G51" s="68">
+        <v>5</v>
+      </c>
+      <c r="H51" s="68">
+        <f>E51</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I51" s="100">
+        <f t="shared" si="8"/>
+        <v>2.55106728462327E-3</v>
+      </c>
+      <c r="J51" s="106">
+        <f t="shared" si="7"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K51" s="101">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L51" s="101">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="N51" s="68" t="s">
+        <v>272</v>
+      </c>
+      <c r="O51" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q51" s="92"/>
+      <c r="R51" s="92"/>
+      <c r="S51" s="92"/>
+    </row>
+    <row r="52" spans="2:19">
+      <c r="B52" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="68" t="s">
+      <c r="C52" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="D49" s="68" t="s">
+      <c r="D52" s="68" t="s">
         <v>273</v>
       </c>
-      <c r="E49" s="68">
+      <c r="E52" s="68">
         <v>4.3200000000000001E-3</v>
       </c>
-      <c r="F49" s="68" t="s">
+      <c r="F52" s="68" t="s">
         <v>249</v>
       </c>
-      <c r="G49" s="68">
+      <c r="G52" s="68">
         <v>5</v>
       </c>
-      <c r="H49" s="68">
-        <f>E49</f>
+      <c r="H52" s="68">
+        <f>E52</f>
         <v>4.3200000000000001E-3</v>
       </c>
-      <c r="I49" s="68">
-        <f>(L49-K49)/(2*NORMINV(0.975,0,1))</f>
+      <c r="I52" s="68">
+        <f t="shared" si="8"/>
         <v>1.4285976793890307E-4</v>
       </c>
-      <c r="J49" s="106">
+      <c r="J52" s="106">
         <f t="shared" si="7"/>
         <v>4.3200000000000001E-3</v>
       </c>
-      <c r="K49" s="68">
+      <c r="K52" s="68">
         <v>4.0400000000000002E-3</v>
       </c>
-      <c r="L49" s="68">
+      <c r="L52" s="68">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="N49" s="68" t="s">
+      <c r="N52" s="68" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:14">
-      <c r="B50" s="68" t="s">
+    <row r="53" spans="2:19">
+      <c r="B53" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="68" t="s">
+      <c r="C53" s="68" t="s">
         <v>274</v>
       </c>
-      <c r="D50" s="68" t="s">
+      <c r="D53" s="68" t="s">
         <v>275</v>
       </c>
-      <c r="E50" s="68">
+      <c r="E53" s="68">
         <v>-0.08</v>
       </c>
-      <c r="F50" s="68" t="s">
+      <c r="F53" s="68" t="s">
         <v>249</v>
       </c>
-      <c r="G50" s="68">
+      <c r="G53" s="68">
         <v>5</v>
       </c>
-      <c r="H50" s="68">
-        <f t="shared" ref="H50:H52" si="8">E50</f>
+      <c r="H53" s="68">
+        <f t="shared" ref="H53:H55" si="9">E53</f>
         <v>-0.08</v>
       </c>
-      <c r="I50" s="68">
-        <f>(L50-K50)/(2*NORMINV(0.975,0,1))</f>
+      <c r="I53" s="68">
+        <f t="shared" si="8"/>
         <v>4.3368143838595594E-2</v>
       </c>
-      <c r="J50" s="106">
-        <f>E50</f>
+      <c r="J53" s="106">
+        <f>E53</f>
         <v>-0.08</v>
       </c>
-      <c r="K50" s="68">
+      <c r="K53" s="68">
         <v>-0.3</v>
       </c>
-      <c r="L50" s="68">
+      <c r="L53" s="68">
         <v>-0.13</v>
       </c>
-      <c r="N50" s="68" t="s">
+      <c r="N53" s="68" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="51" spans="2:14">
-      <c r="B51" s="68" t="s">
+    <row r="54" spans="2:19">
+      <c r="B54" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="C51" s="68" t="s">
-        <v>320</v>
-      </c>
-      <c r="D51" s="68" t="s">
+      <c r="C54" s="68" t="s">
+        <v>318</v>
+      </c>
+      <c r="D54" s="68" t="s">
         <v>277</v>
       </c>
-      <c r="E51" s="68">
+      <c r="E54" s="68">
         <v>-0.18</v>
       </c>
-      <c r="F51" s="68" t="s">
+      <c r="F54" s="68" t="s">
         <v>249</v>
       </c>
-      <c r="G51" s="68">
+      <c r="G54" s="68">
         <v>5</v>
       </c>
-      <c r="H51" s="68">
+      <c r="H54" s="68">
+        <f t="shared" si="9"/>
+        <v>-0.18</v>
+      </c>
+      <c r="I54" s="68">
         <f t="shared" si="8"/>
-        <v>-0.18</v>
-      </c>
-      <c r="I51" s="68">
-        <f>(L51-K51)/(2*NORMINV(0.975,0,1))</f>
         <v>6.1225614830958487E-2</v>
       </c>
-      <c r="J51" s="106">
+      <c r="J54" s="106">
         <f t="shared" si="7"/>
         <v>-0.18</v>
       </c>
-      <c r="K51" s="68">
+      <c r="K54" s="68">
         <v>-0.3</v>
       </c>
-      <c r="L51" s="68">
+      <c r="L54" s="68">
         <v>-0.06</v>
       </c>
-      <c r="N51" s="68" t="s">
+      <c r="N54" s="68" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="52" spans="2:14">
-      <c r="B52" s="68" t="s">
+    <row r="55" spans="2:19">
+      <c r="B55" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="68" t="s">
+      <c r="C55" s="68" t="s">
         <v>279</v>
       </c>
-      <c r="D52" s="68" t="s">
+      <c r="D55" s="68" t="s">
         <v>280</v>
       </c>
-      <c r="E52" s="68">
+      <c r="E55" s="68">
         <v>0</v>
       </c>
-      <c r="F52" s="68" t="s">
+      <c r="F55" s="68" t="s">
         <v>242</v>
       </c>
-      <c r="G52" s="68">
+      <c r="G55" s="68">
         <v>6</v>
       </c>
-      <c r="H52" s="68">
-        <f t="shared" si="8"/>
+      <c r="H55" s="68">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I52" s="68">
-        <f t="shared" ref="I52" si="9">(L52-K52)/(2*NORMINV(0.975,0,1))</f>
+      <c r="I55" s="68">
+        <f t="shared" ref="I55" si="10">(L55-K55)/(2*NORMINV(0.975,0,1))</f>
         <v>0</v>
       </c>
-      <c r="J52" s="106">
+      <c r="J55" s="106">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K52" s="68">
+      <c r="K55" s="68">
         <v>0</v>
       </c>
-      <c r="L52" s="68">
+      <c r="L55" s="68">
         <v>0</v>
       </c>
-      <c r="N52" s="68" t="s">
+      <c r="N55" s="68" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="53" spans="2:14">
-      <c r="B53" s="68" t="s">
+    <row r="56" spans="2:19">
+      <c r="B56" s="68" t="s">
         <v>281</v>
       </c>
-      <c r="C53" s="68" t="s">
+      <c r="C56" s="68" t="s">
         <v>282</v>
       </c>
-      <c r="D53" s="68" t="s">
+      <c r="D56" s="68" t="s">
         <v>283</v>
       </c>
-      <c r="E53" s="68">
-        <v>610.58000000000004</v>
-      </c>
-      <c r="F53" s="68" t="s">
+      <c r="E56" s="68">
+        <v>612.14</v>
+      </c>
+      <c r="F56" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="G53" s="68">
+      <c r="G56" s="68">
         <v>2</v>
       </c>
-      <c r="H53" s="68">
+      <c r="H56" s="68">
         <v>100</v>
       </c>
-      <c r="I53" s="68">
-        <f>E53/H53</f>
-        <v>6.1058000000000003</v>
-      </c>
-      <c r="J53" s="106">
+      <c r="I56" s="68">
+        <f>E56/H56</f>
+        <v>6.1213999999999995</v>
+      </c>
+      <c r="J56" s="106">
         <f t="shared" si="7"/>
-        <v>610.58000000000004</v>
-      </c>
-      <c r="K53" s="68">
-        <f>_xlfn.GAMMA.INV(0.025,H53,I53)</f>
-        <v>496.79225777988648</v>
-      </c>
-      <c r="L53" s="68">
-        <f>_xlfn.GAMMA.INV(0.975,H53,I53)</f>
-        <v>735.92564919121662</v>
-      </c>
-      <c r="N53" s="68" t="s">
+        <v>612.14</v>
+      </c>
+      <c r="K56" s="68">
+        <f>_xlfn.GAMMA.INV(0.025,H56,I56)</f>
+        <v>498.06153604340085</v>
+      </c>
+      <c r="L56" s="68">
+        <f>_xlfn.GAMMA.INV(0.975,H56,I56)</f>
+        <v>737.80590077616569</v>
+      </c>
+      <c r="N56" s="68" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="54" spans="2:14">
-      <c r="B54" s="68" t="s">
+    <row r="57" spans="2:19">
+      <c r="B57" s="68" t="s">
         <v>281</v>
       </c>
-      <c r="C54" s="68" t="s">
+      <c r="C57" s="68" t="s">
+        <v>354</v>
+      </c>
+      <c r="D57" s="68" t="s">
+        <v>355</v>
+      </c>
+      <c r="E57" s="68">
+        <v>135.38999999999999</v>
+      </c>
+      <c r="F57" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="G57" s="68">
+        <v>2</v>
+      </c>
+      <c r="H57" s="68">
+        <v>100</v>
+      </c>
+      <c r="I57" s="68">
+        <f>E57/H57</f>
+        <v>1.3538999999999999</v>
+      </c>
+      <c r="J57" s="106">
+        <f t="shared" si="7"/>
+        <v>135.38999999999999</v>
+      </c>
+      <c r="K57" s="68">
+        <f>_xlfn.GAMMA.INV(0.025,H57,I57)</f>
+        <v>110.15870775462483</v>
+      </c>
+      <c r="L57" s="68">
+        <f>_xlfn.GAMMA.INV(0.975,H57,I57)</f>
+        <v>163.18414236299714</v>
+      </c>
+      <c r="N57" s="68" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="58" spans="2:19" s="117" customFormat="1">
+      <c r="B58" s="117" t="s">
+        <v>281</v>
+      </c>
+      <c r="C58" s="117" t="s">
+        <v>357</v>
+      </c>
+      <c r="D58" s="117" t="s">
+        <v>356</v>
+      </c>
+      <c r="E58" s="117">
+        <v>534.96</v>
+      </c>
+      <c r="F58" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="G58" s="117">
+        <v>2</v>
+      </c>
+      <c r="H58" s="117">
+        <v>100</v>
+      </c>
+      <c r="I58" s="117">
+        <f>E58/H58</f>
+        <v>5.3496000000000006</v>
+      </c>
+      <c r="J58" s="117">
+        <f t="shared" ref="J58" si="11">E58</f>
+        <v>534.96</v>
+      </c>
+      <c r="K58" s="117">
+        <f>_xlfn.GAMMA.INV(0.025,H58,I58)</f>
+        <v>435.26480759593846</v>
+      </c>
+      <c r="L58" s="117">
+        <f>_xlfn.GAMMA.INV(0.975,H58,I58)</f>
+        <v>644.78165890028049</v>
+      </c>
+    </row>
+    <row r="59" spans="2:19">
+      <c r="B59" s="68" t="s">
+        <v>281</v>
+      </c>
+      <c r="C59" s="68" t="s">
         <v>285</v>
       </c>
-      <c r="D54" s="68" t="s">
+      <c r="D59" s="68" t="s">
         <v>286</v>
       </c>
-      <c r="E54" s="68">
-        <v>584.89</v>
-      </c>
-      <c r="F54" s="68" t="s">
+      <c r="E59" s="68">
+        <v>2348.8000000000002</v>
+      </c>
+      <c r="F59" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="G54" s="68">
+      <c r="G59" s="68">
         <v>2</v>
       </c>
-      <c r="H54" s="68">
+      <c r="H59" s="68">
         <v>100</v>
       </c>
-      <c r="I54" s="68">
-        <f>E54/H54</f>
-        <v>5.8488999999999995</v>
-      </c>
-      <c r="J54" s="106">
-        <f t="shared" si="7"/>
-        <v>584.89</v>
-      </c>
-      <c r="K54" s="68">
-        <f>_xlfn.GAMMA.INV(0.025,H54,I54)</f>
-        <v>475.88984842752427</v>
-      </c>
-      <c r="L54" s="68">
-        <f>_xlfn.GAMMA.INV(0.975,H54,I54)</f>
-        <v>704.96176251343081</v>
-      </c>
-      <c r="N54" s="68" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="55" spans="2:14">
-      <c r="B55" s="68" t="s">
-        <v>281</v>
-      </c>
-      <c r="C55" s="68" t="s">
-        <v>287</v>
-      </c>
-      <c r="D55" s="68" t="s">
-        <v>288</v>
-      </c>
-      <c r="E55" s="68">
-        <v>2348.8000000000002</v>
-      </c>
-      <c r="F55" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="G55" s="68">
-        <v>2</v>
-      </c>
-      <c r="H55" s="68">
-        <v>100</v>
-      </c>
-      <c r="I55" s="68">
-        <f>E55/H55</f>
+      <c r="I59" s="68">
+        <f>E59/H59</f>
         <v>23.488000000000003</v>
       </c>
-      <c r="J55" s="106">
+      <c r="J59" s="106">
         <f t="shared" si="7"/>
         <v>2348.8000000000002</v>
       </c>
-      <c r="K55" s="68">
-        <f>_xlfn.GAMMA.INV(0.025,H55,I55)</f>
+      <c r="K59" s="68">
+        <f>_xlfn.GAMMA.INV(0.025,H59,I59)</f>
         <v>1911.0774265016828</v>
       </c>
-      <c r="L55" s="68">
-        <f t="shared" ref="L55" si="10">_xlfn.GAMMA.INV(0.975,H55,I55)</f>
+      <c r="L59" s="68">
+        <f t="shared" ref="L59" si="12">_xlfn.GAMMA.INV(0.975,H59,I59)</f>
         <v>2830.9839248261155</v>
       </c>
-      <c r="M55" s="91"/>
-      <c r="N55" s="68" t="s">
+      <c r="M59" s="91"/>
+      <c r="N59" s="68" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="56" spans="2:14">
-      <c r="B56" s="68" t="s">
+    <row r="60" spans="2:19">
+      <c r="B60" s="68" t="s">
         <v>281</v>
       </c>
-      <c r="C56" s="68" t="s">
-        <v>289</v>
-      </c>
-      <c r="D56" s="68" t="s">
-        <v>290</v>
-      </c>
-      <c r="E56" s="68">
+      <c r="C60" s="68" t="s">
+        <v>287</v>
+      </c>
+      <c r="D60" s="68" t="s">
+        <v>288</v>
+      </c>
+      <c r="E60" s="68">
         <v>-57.2</v>
       </c>
-      <c r="F56" s="68" t="s">
+      <c r="F60" s="68" t="s">
         <v>249</v>
       </c>
-      <c r="G56" s="68">
+      <c r="G60" s="68">
         <v>5</v>
       </c>
-      <c r="H56" s="68">
-        <f>E56</f>
+      <c r="H60" s="68">
+        <f>E60</f>
         <v>-57.2</v>
       </c>
-      <c r="I56" s="68">
-        <f>-E56*0.1</f>
+      <c r="I60" s="68">
+        <f>-E60*0.1</f>
         <v>5.7200000000000006</v>
       </c>
-      <c r="J56" s="106">
+      <c r="J60" s="106">
         <f t="shared" si="7"/>
         <v>-57.2</v>
       </c>
-      <c r="K56" s="68">
-        <f>E56-(I56*NORMINV(0.975,0,1))</f>
+      <c r="K60" s="68">
+        <f>E60-(I60*NORMINV(0.975,0,1))</f>
         <v>-68.410993991569114</v>
       </c>
-      <c r="L56" s="68">
-        <f>E56+(I56*NORMINV(0.975,0,1))</f>
+      <c r="L60" s="68">
+        <f>E60+(I60*NORMINV(0.975,0,1))</f>
         <v>-45.989006008430891</v>
       </c>
-      <c r="N56" s="68" t="s">
+      <c r="N60" s="68" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="57" spans="2:14">
-      <c r="B57" s="68" t="s">
+    <row r="61" spans="2:19">
+      <c r="B61" s="68" t="s">
         <v>281</v>
       </c>
-      <c r="C57" s="68" t="s">
-        <v>291</v>
-      </c>
-      <c r="D57" s="68" t="s">
-        <v>292</v>
-      </c>
-      <c r="E57" s="68">
+      <c r="C61" s="68" t="s">
+        <v>289</v>
+      </c>
+      <c r="D61" s="68" t="s">
+        <v>290</v>
+      </c>
+      <c r="E61" s="68">
         <v>-242</v>
       </c>
-      <c r="F57" s="68" t="s">
+      <c r="F61" s="68" t="s">
         <v>249</v>
       </c>
-      <c r="G57" s="68">
+      <c r="G61" s="68">
         <v>5</v>
       </c>
-      <c r="H57" s="68">
-        <f t="shared" ref="H57:H58" si="11">E57</f>
+      <c r="H61" s="68">
+        <f t="shared" ref="H61:H62" si="13">E61</f>
         <v>-242</v>
       </c>
-      <c r="I57" s="68">
-        <f>-E57*0.1</f>
+      <c r="I61" s="68">
+        <f>-E61*0.1</f>
         <v>24.200000000000003</v>
       </c>
-      <c r="J57" s="106">
+      <c r="J61" s="106">
         <f t="shared" si="7"/>
         <v>-242</v>
       </c>
-      <c r="K57" s="68">
-        <f>E57-(I57*NORMINV(0.975,0,1))</f>
+      <c r="K61" s="68">
+        <f>E61-(I61*NORMINV(0.975,0,1))</f>
         <v>-289.4311284258693</v>
       </c>
-      <c r="L57" s="68">
-        <f>E57+(I57*NORMINV(0.975,0,1))</f>
+      <c r="L61" s="68">
+        <f>E61+(I61*NORMINV(0.975,0,1))</f>
         <v>-194.5688715741307</v>
       </c>
-      <c r="N57" s="68" t="s">
+      <c r="N61" s="68" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="58" spans="2:14">
-      <c r="B58" s="68" t="s">
+    <row r="62" spans="2:19">
+      <c r="B62" s="68" t="s">
         <v>281</v>
       </c>
-      <c r="C58" s="68" t="s">
+      <c r="C62" s="68" t="s">
+        <v>291</v>
+      </c>
+      <c r="D62" s="68" t="s">
+        <v>292</v>
+      </c>
+      <c r="E62" s="68">
+        <v>-921.4</v>
+      </c>
+      <c r="F62" s="68" t="s">
+        <v>249</v>
+      </c>
+      <c r="G62" s="68">
+        <v>5</v>
+      </c>
+      <c r="H62" s="68">
+        <f t="shared" si="13"/>
+        <v>-921.4</v>
+      </c>
+      <c r="I62" s="68">
+        <f>-E62*0.1</f>
+        <v>92.14</v>
+      </c>
+      <c r="J62" s="106">
+        <f>E62</f>
+        <v>-921.4</v>
+      </c>
+      <c r="K62" s="68">
+        <f>E62-(I62*NORMINV(0.975,0,1))</f>
+        <v>-1101.9910815355206</v>
+      </c>
+      <c r="L62" s="68">
+        <f>E62+(I62*NORMINV(0.975,0,1))</f>
+        <v>-740.80891846447946</v>
+      </c>
+      <c r="N62" s="68" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="63" spans="2:19">
+      <c r="B63" s="68" t="s">
+        <v>281</v>
+      </c>
+      <c r="C63" s="68" t="s">
         <v>293</v>
       </c>
-      <c r="D58" s="68" t="s">
+      <c r="D63" s="68" t="s">
         <v>294</v>
       </c>
-      <c r="E58" s="68">
-        <v>-921.4</v>
-      </c>
-      <c r="F58" s="68" t="s">
+      <c r="E63" s="68">
+        <v>-1514</v>
+      </c>
+      <c r="F63" s="68" t="s">
         <v>249</v>
       </c>
-      <c r="G58" s="68">
+      <c r="G63" s="68">
         <v>5</v>
       </c>
-      <c r="H58" s="68">
-        <f t="shared" si="11"/>
-        <v>-921.4</v>
-      </c>
-      <c r="I58" s="68">
-        <f>-E58*0.1</f>
-        <v>92.14</v>
-      </c>
-      <c r="J58" s="106">
-        <f>E58</f>
-        <v>-921.4</v>
-      </c>
-      <c r="K58" s="68">
-        <f>E58-(I58*NORMINV(0.975,0,1))</f>
-        <v>-1101.9910815355206</v>
-      </c>
-      <c r="L58" s="68">
-        <f>E58+(I58*NORMINV(0.975,0,1))</f>
-        <v>-740.80891846447946</v>
-      </c>
-      <c r="N58" s="68" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="59" spans="2:14">
-      <c r="B59" s="68" t="s">
-        <v>281</v>
-      </c>
-      <c r="C59" s="68" t="s">
-        <v>295</v>
-      </c>
-      <c r="D59" s="68" t="s">
-        <v>296</v>
-      </c>
-      <c r="E59" s="68">
+      <c r="H63" s="68">
+        <f>E63</f>
         <v>-1514</v>
       </c>
-      <c r="F59" s="68" t="s">
-        <v>249</v>
-      </c>
-      <c r="G59" s="68">
-        <v>5</v>
-      </c>
-      <c r="H59" s="68">
-        <f>E59</f>
-        <v>-1514</v>
-      </c>
-      <c r="I59" s="68">
-        <f>-E59*0.1</f>
+      <c r="I63" s="68">
+        <f>-E63*0.1</f>
         <v>151.4</v>
       </c>
-      <c r="J59" s="106">
+      <c r="J63" s="106">
         <f t="shared" si="7"/>
         <v>-1514</v>
       </c>
-      <c r="K59" s="68">
-        <f>E59-(I59*NORMINV(0.975,0,1))</f>
+      <c r="K63" s="68">
+        <f>E63-(I63*NORMINV(0.975,0,1))</f>
         <v>-1810.7385472593642</v>
       </c>
-      <c r="L59" s="68">
-        <f>E59+(I59*NORMINV(0.975,0,1))</f>
+      <c r="L63" s="68">
+        <f>E63+(I63*NORMINV(0.975,0,1))</f>
         <v>-1217.2614527406358</v>
       </c>
-      <c r="N59" s="68" t="s">
+      <c r="N63" s="68" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="60" spans="2:14">
-      <c r="B60" s="68" t="s">
+    <row r="64" spans="2:19">
+      <c r="B64" s="68" t="s">
         <v>281</v>
       </c>
-      <c r="C60" s="68" t="s">
-        <v>297</v>
-      </c>
-      <c r="D60" s="68" t="s">
-        <v>298</v>
-      </c>
-      <c r="E60" s="68">
+      <c r="C64" s="68" t="s">
+        <v>295</v>
+      </c>
+      <c r="D64" s="68" t="s">
+        <v>296</v>
+      </c>
+      <c r="E64" s="68">
         <v>1446.8</v>
       </c>
-      <c r="F60" s="68" t="s">
+      <c r="F64" s="68" t="s">
         <v>249</v>
       </c>
-      <c r="G60" s="68">
+      <c r="G64" s="68">
         <v>5</v>
       </c>
-      <c r="H60" s="68">
-        <f>E60</f>
+      <c r="H64" s="68">
+        <f>E64</f>
         <v>1446.8</v>
       </c>
-      <c r="I60" s="100">
-        <f>H60*0.1</f>
+      <c r="I64" s="100">
+        <f>H64*0.1</f>
         <v>144.68</v>
       </c>
-      <c r="J60" s="106">
+      <c r="J64" s="106">
         <f t="shared" si="7"/>
         <v>1446.8</v>
       </c>
-      <c r="K60" s="101">
-        <f>E60-(I60*NORMINV(0.975,0,1))</f>
+      <c r="K64" s="101">
+        <f>E64-(I64*NORMINV(0.975,0,1))</f>
         <v>1163.2324107167451</v>
       </c>
-      <c r="L60" s="101">
-        <f>E60+(I60*NORMINV(0.975,0,1))</f>
+      <c r="L64" s="101">
+        <f>E64+(I64*NORMINV(0.975,0,1))</f>
         <v>1730.3675892832548</v>
-      </c>
-      <c r="N60" s="68" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="61" spans="2:14">
-      <c r="B61" s="68" t="s">
-        <v>281</v>
-      </c>
-      <c r="C61" s="68" t="s">
-        <v>299</v>
-      </c>
-      <c r="D61" s="68" t="s">
-        <v>300</v>
-      </c>
-      <c r="E61" s="68">
-        <v>1676.1</v>
-      </c>
-      <c r="F61" s="68" t="s">
-        <v>249</v>
-      </c>
-      <c r="G61" s="68">
-        <v>5</v>
-      </c>
-      <c r="H61" s="68">
-        <f t="shared" ref="H61:H64" si="12">E61</f>
-        <v>1676.1</v>
-      </c>
-      <c r="I61" s="100">
-        <f>H61*0.1</f>
-        <v>167.61</v>
-      </c>
-      <c r="J61" s="106">
-        <f t="shared" si="7"/>
-        <v>1676.1</v>
-      </c>
-      <c r="K61" s="101">
-        <f t="shared" ref="K61:K64" si="13">E61-(I61*NORMINV(0.975,0,1))</f>
-        <v>1347.5904365512415</v>
-      </c>
-      <c r="L61" s="101">
-        <f t="shared" ref="L61:L64" si="14">E61+(I61*NORMINV(0.975,0,1))</f>
-        <v>2004.6095634487583</v>
-      </c>
-      <c r="N61" s="68" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="62" spans="2:14">
-      <c r="B62" s="68" t="s">
-        <v>281</v>
-      </c>
-      <c r="C62" s="68" t="s">
-        <v>301</v>
-      </c>
-      <c r="D62" s="68" t="s">
-        <v>302</v>
-      </c>
-      <c r="E62" s="68">
-        <v>3956.7</v>
-      </c>
-      <c r="F62" s="68" t="s">
-        <v>249</v>
-      </c>
-      <c r="G62" s="68">
-        <v>5</v>
-      </c>
-      <c r="H62" s="68">
-        <f t="shared" si="12"/>
-        <v>3956.7</v>
-      </c>
-      <c r="I62" s="100">
-        <f t="shared" ref="I62:I64" si="15">H62*0.1</f>
-        <v>395.67</v>
-      </c>
-      <c r="J62" s="106">
-        <f t="shared" si="7"/>
-        <v>3956.7</v>
-      </c>
-      <c r="K62" s="101">
-        <f t="shared" si="13"/>
-        <v>3181.2010502370367</v>
-      </c>
-      <c r="L62" s="101">
-        <f t="shared" si="14"/>
-        <v>4732.1989497629629</v>
-      </c>
-      <c r="N62" s="68" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="63" spans="2:14">
-      <c r="B63" s="68" t="s">
-        <v>281</v>
-      </c>
-      <c r="C63" s="68" t="s">
-        <v>303</v>
-      </c>
-      <c r="D63" s="68" t="s">
-        <v>304</v>
-      </c>
-      <c r="E63" s="68">
-        <v>5406.9</v>
-      </c>
-      <c r="F63" s="68" t="s">
-        <v>249</v>
-      </c>
-      <c r="G63" s="68">
-        <v>5</v>
-      </c>
-      <c r="H63" s="68">
-        <f t="shared" si="12"/>
-        <v>5406.9</v>
-      </c>
-      <c r="I63" s="100">
-        <f t="shared" si="15"/>
-        <v>540.68999999999994</v>
-      </c>
-      <c r="J63" s="106">
-        <f t="shared" si="7"/>
-        <v>5406.9</v>
-      </c>
-      <c r="K63" s="101">
-        <f t="shared" si="13"/>
-        <v>4347.167073199038</v>
-      </c>
-      <c r="L63" s="101">
-        <f t="shared" si="14"/>
-        <v>6466.6329268009613</v>
-      </c>
-      <c r="N63" s="68" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="64" spans="2:14">
-      <c r="B64" s="68" t="s">
-        <v>281</v>
-      </c>
-      <c r="C64" s="68" t="s">
-        <v>305</v>
-      </c>
-      <c r="D64" s="68" t="s">
-        <v>306</v>
-      </c>
-      <c r="E64" s="68">
-        <v>1217.4000000000001</v>
-      </c>
-      <c r="F64" s="68" t="s">
-        <v>249</v>
-      </c>
-      <c r="G64" s="68">
-        <v>5</v>
-      </c>
-      <c r="H64" s="68">
-        <f t="shared" si="12"/>
-        <v>1217.4000000000001</v>
-      </c>
-      <c r="I64" s="100">
-        <f t="shared" si="15"/>
-        <v>121.74000000000001</v>
-      </c>
-      <c r="J64" s="106">
-        <f t="shared" si="7"/>
-        <v>1217.4000000000001</v>
-      </c>
-      <c r="K64" s="101">
-        <f t="shared" si="13"/>
-        <v>978.79398452209398</v>
-      </c>
-      <c r="L64" s="101">
-        <f t="shared" si="14"/>
-        <v>1456.0060154779062</v>
       </c>
       <c r="N64" s="68" t="s">
         <v>278</v>
@@ -6294,181 +6398,185 @@
         <v>281</v>
       </c>
       <c r="C65" s="68" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="D65" s="68" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
       <c r="E65" s="68">
-        <v>401</v>
+        <v>1676.1</v>
       </c>
       <c r="F65" s="68" t="s">
-        <v>47</v>
+        <v>249</v>
       </c>
       <c r="G65" s="68">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H65" s="68">
-        <v>100</v>
+        <f t="shared" ref="H65:H68" si="14">E65</f>
+        <v>1676.1</v>
       </c>
       <c r="I65" s="100">
-        <f>E65/H65</f>
-        <v>4.01</v>
+        <f>H65*0.1</f>
+        <v>167.61</v>
       </c>
       <c r="J65" s="106">
         <f t="shared" si="7"/>
-        <v>401</v>
+        <v>1676.1</v>
       </c>
       <c r="K65" s="101">
-        <f>_xlfn.GAMMA.INV(0.025,H65,I65)</f>
-        <v>326.26960491620173</v>
+        <f t="shared" ref="K65:K68" si="15">E65-(I65*NORMINV(0.975,0,1))</f>
+        <v>1347.5904365512415</v>
       </c>
       <c r="L65" s="101">
-        <f>_xlfn.GAMMA.INV(0.975,H65,I65)</f>
-        <v>483.32108049015335</v>
+        <f t="shared" ref="L65:L68" si="16">E65+(I65*NORMINV(0.975,0,1))</f>
+        <v>2004.6095634487583</v>
       </c>
       <c r="N65" s="68" t="s">
-        <v>308</v>
+        <v>278</v>
       </c>
     </row>
     <row r="66" spans="2:14">
       <c r="B66" s="68" t="s">
-        <v>309</v>
+        <v>281</v>
       </c>
       <c r="C66" s="68" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="D66" s="68" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="E66" s="68">
-        <v>8.57</v>
+        <v>3956.7</v>
       </c>
       <c r="F66" s="68" t="s">
-        <v>47</v>
+        <v>249</v>
       </c>
       <c r="G66" s="68">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H66" s="68">
-        <v>100</v>
-      </c>
-      <c r="I66" s="68">
-        <f>E66/H66</f>
-        <v>8.5699999999999998E-2</v>
+        <f t="shared" si="14"/>
+        <v>3956.7</v>
+      </c>
+      <c r="I66" s="100">
+        <f t="shared" ref="I66:I68" si="17">H66*0.1</f>
+        <v>395.67</v>
       </c>
       <c r="J66" s="106">
         <f t="shared" si="7"/>
-        <v>8.57</v>
+        <v>3956.7</v>
       </c>
       <c r="K66" s="101">
-        <f t="shared" ref="K66:K69" si="16">_xlfn.GAMMA.INV(0.025,H66,I66)</f>
-        <v>6.9728940502041121</v>
+        <f t="shared" si="15"/>
+        <v>3181.2010502370367</v>
       </c>
       <c r="L66" s="101">
-        <f t="shared" ref="L66:L69" si="17">_xlfn.GAMMA.INV(0.975,H66,I66)</f>
-        <v>10.329330822445423</v>
+        <f t="shared" si="16"/>
+        <v>4732.1989497629629</v>
       </c>
       <c r="N66" s="68" t="s">
-        <v>311</v>
+        <v>278</v>
       </c>
     </row>
     <row r="67" spans="2:14">
       <c r="B67" s="68" t="s">
-        <v>309</v>
+        <v>281</v>
       </c>
       <c r="C67" s="68" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="D67" s="68" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="E67" s="68">
-        <v>1.3</v>
+        <v>5406.9</v>
       </c>
       <c r="F67" s="68" t="s">
-        <v>47</v>
+        <v>249</v>
       </c>
       <c r="G67" s="68">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H67" s="68">
-        <v>100</v>
-      </c>
-      <c r="I67" s="68">
-        <f>E67/H67</f>
-        <v>1.3000000000000001E-2</v>
+        <f t="shared" si="14"/>
+        <v>5406.9</v>
+      </c>
+      <c r="I67" s="100">
+        <f t="shared" si="17"/>
+        <v>540.68999999999994</v>
       </c>
       <c r="J67" s="106">
         <f t="shared" si="7"/>
-        <v>1.3</v>
+        <v>5406.9</v>
       </c>
       <c r="K67" s="101">
+        <f t="shared" si="15"/>
+        <v>4347.167073199038</v>
+      </c>
+      <c r="L67" s="101">
         <f t="shared" si="16"/>
-        <v>1.0577318862620009</v>
-      </c>
-      <c r="L67" s="101">
-        <f t="shared" si="17"/>
-        <v>1.566876320791021</v>
+        <v>6466.6329268009613</v>
       </c>
       <c r="N67" s="68" t="s">
-        <v>311</v>
+        <v>278</v>
       </c>
     </row>
     <row r="68" spans="2:14">
       <c r="B68" s="68" t="s">
-        <v>309</v>
+        <v>281</v>
       </c>
       <c r="C68" s="68" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="D68" s="68" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="E68" s="68">
-        <v>11.8</v>
+        <v>1217.4000000000001</v>
       </c>
       <c r="F68" s="68" t="s">
-        <v>47</v>
+        <v>249</v>
       </c>
       <c r="G68" s="68">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H68" s="68">
-        <v>100</v>
-      </c>
-      <c r="I68" s="68">
-        <f t="shared" ref="I68:I69" si="18">E68/H68</f>
-        <v>0.11800000000000001</v>
+        <f t="shared" si="14"/>
+        <v>1217.4000000000001</v>
+      </c>
+      <c r="I68" s="100">
+        <f t="shared" si="17"/>
+        <v>121.74000000000001</v>
       </c>
       <c r="J68" s="106">
         <f t="shared" si="7"/>
-        <v>11.8</v>
+        <v>1217.4000000000001</v>
       </c>
       <c r="K68" s="101">
+        <f t="shared" si="15"/>
+        <v>978.79398452209398</v>
+      </c>
+      <c r="L68" s="101">
         <f t="shared" si="16"/>
-        <v>9.6009509676089309</v>
-      </c>
-      <c r="L68" s="101">
-        <f t="shared" si="17"/>
-        <v>14.222415834872344</v>
+        <v>1456.0060154779062</v>
       </c>
       <c r="N68" s="68" t="s">
-        <v>311</v>
+        <v>278</v>
       </c>
     </row>
     <row r="69" spans="2:14">
       <c r="B69" s="68" t="s">
-        <v>309</v>
+        <v>281</v>
       </c>
       <c r="C69" s="68" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="D69" s="68" t="s">
         <v>317</v>
       </c>
       <c r="E69" s="68">
-        <v>3.86</v>
+        <v>401</v>
       </c>
       <c r="F69" s="68" t="s">
         <v>47</v>
@@ -6479,24 +6587,210 @@
       <c r="H69" s="68">
         <v>100</v>
       </c>
-      <c r="I69" s="68">
-        <f t="shared" si="18"/>
-        <v>3.8599999999999995E-2</v>
+      <c r="I69" s="100">
+        <f>E69/H69</f>
+        <v>4.01</v>
       </c>
       <c r="J69" s="106">
         <f t="shared" si="7"/>
+        <v>401</v>
+      </c>
+      <c r="K69" s="101">
+        <f>_xlfn.GAMMA.INV(0.025,H69,I69)</f>
+        <v>326.26960491620173</v>
+      </c>
+      <c r="L69" s="101">
+        <f>_xlfn.GAMMA.INV(0.975,H69,I69)</f>
+        <v>483.32108049015335</v>
+      </c>
+      <c r="N69" s="68" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="70" spans="2:14">
+      <c r="B70" s="68" t="s">
+        <v>307</v>
+      </c>
+      <c r="C70" s="68" t="s">
+        <v>308</v>
+      </c>
+      <c r="D70" s="68" t="s">
+        <v>316</v>
+      </c>
+      <c r="E70" s="68">
+        <v>8.57</v>
+      </c>
+      <c r="F70" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="G70" s="68">
+        <v>2</v>
+      </c>
+      <c r="H70" s="68">
+        <v>100</v>
+      </c>
+      <c r="I70" s="68">
+        <f>E70/H70</f>
+        <v>8.5699999999999998E-2</v>
+      </c>
+      <c r="J70" s="106">
+        <f t="shared" si="7"/>
+        <v>8.57</v>
+      </c>
+      <c r="K70" s="101">
+        <f t="shared" ref="K70:K73" si="18">_xlfn.GAMMA.INV(0.025,H70,I70)</f>
+        <v>6.9728940502041121</v>
+      </c>
+      <c r="L70" s="101">
+        <f t="shared" ref="L70:L73" si="19">_xlfn.GAMMA.INV(0.975,H70,I70)</f>
+        <v>10.329330822445423</v>
+      </c>
+      <c r="N70" s="68" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14">
+      <c r="B71" s="68" t="s">
+        <v>307</v>
+      </c>
+      <c r="C71" s="68" t="s">
+        <v>310</v>
+      </c>
+      <c r="D71" s="68" t="s">
+        <v>311</v>
+      </c>
+      <c r="E71" s="68">
+        <v>1.3</v>
+      </c>
+      <c r="F71" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="G71" s="68">
+        <v>2</v>
+      </c>
+      <c r="H71" s="68">
+        <v>100</v>
+      </c>
+      <c r="I71" s="68">
+        <f>E71/H71</f>
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="J71" s="106">
+        <f t="shared" si="7"/>
+        <v>1.3</v>
+      </c>
+      <c r="K71" s="101">
+        <f t="shared" si="18"/>
+        <v>1.0577318862620009</v>
+      </c>
+      <c r="L71" s="101">
+        <f t="shared" si="19"/>
+        <v>1.566876320791021</v>
+      </c>
+      <c r="N71" s="68" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="72" spans="2:14">
+      <c r="B72" s="68" t="s">
+        <v>307</v>
+      </c>
+      <c r="C72" s="68" t="s">
+        <v>312</v>
+      </c>
+      <c r="D72" s="68" t="s">
+        <v>313</v>
+      </c>
+      <c r="E72" s="68">
+        <v>11.8</v>
+      </c>
+      <c r="F72" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="G72" s="68">
+        <v>2</v>
+      </c>
+      <c r="H72" s="68">
+        <v>100</v>
+      </c>
+      <c r="I72" s="68">
+        <f t="shared" ref="I72:I73" si="20">E72/H72</f>
+        <v>0.11800000000000001</v>
+      </c>
+      <c r="J72" s="106">
+        <f t="shared" si="7"/>
+        <v>11.8</v>
+      </c>
+      <c r="K72" s="101">
+        <f t="shared" si="18"/>
+        <v>9.6009509676089309</v>
+      </c>
+      <c r="L72" s="101">
+        <f t="shared" si="19"/>
+        <v>14.222415834872344</v>
+      </c>
+      <c r="N72" s="68" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="73" spans="2:14">
+      <c r="B73" s="68" t="s">
+        <v>307</v>
+      </c>
+      <c r="C73" s="68" t="s">
+        <v>314</v>
+      </c>
+      <c r="D73" s="68" t="s">
+        <v>315</v>
+      </c>
+      <c r="E73" s="68">
         <v>3.86</v>
       </c>
-      <c r="K69" s="101">
-        <f t="shared" si="16"/>
+      <c r="F73" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="G73" s="68">
+        <v>2</v>
+      </c>
+      <c r="H73" s="68">
+        <v>100</v>
+      </c>
+      <c r="I73" s="68">
+        <f t="shared" si="20"/>
+        <v>3.8599999999999995E-2</v>
+      </c>
+      <c r="J73" s="106">
+        <f t="shared" si="7"/>
+        <v>3.86</v>
+      </c>
+      <c r="K73" s="101">
+        <f t="shared" si="18"/>
         <v>3.1406500622856326</v>
       </c>
-      <c r="L69" s="101">
-        <f t="shared" si="17"/>
+      <c r="L73" s="101">
+        <f t="shared" si="19"/>
         <v>4.6524173832717999</v>
       </c>
-      <c r="N69" s="68" t="s">
-        <v>308</v>
+      <c r="N73" s="68" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14">
+      <c r="B74" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="68" t="s">
+        <v>372</v>
+      </c>
+      <c r="E74" s="68">
+        <v>0.08</v>
+      </c>
+      <c r="J74" s="106">
+        <f t="shared" si="7"/>
+        <v>0.08</v>
+      </c>
+      <c r="N74" s="120" t="s">
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -6504,6 +6798,7 @@
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="K1:L1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N7" r:id="rId1" xr:uid="{5CDCCDC3-40CB-48A9-AFA2-5C786527191C}"/>
     <hyperlink ref="N8" r:id="rId2" xr:uid="{B4CC6DFF-4B5F-49E1-934E-4758C77C42C5}"/>
@@ -6516,10 +6811,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F32D2E0-32A8-4C75-8C98-9C12E5C1268D}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:F70"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6549,7 +6844,7 @@
         <v>40</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -7403,7 +7698,7 @@
       </c>
       <c r="E34" s="114">
         <f>parameters!I34</f>
-        <v>3.5350227786655028E-3</v>
+        <v>3.5350227786655002E-3</v>
       </c>
       <c r="F34" s="114">
         <f>parameters!J34</f>
@@ -7751,11 +8046,11 @@
     <row r="48" spans="1:6">
       <c r="A48" s="5" t="str">
         <f>parameters!D48</f>
-        <v>Mort.TURBT</v>
+        <v>Sens.joined.diag.HG</v>
       </c>
       <c r="B48" s="113">
         <f>parameters!E48</f>
-        <v>8.0000000000000002E-3</v>
+        <v>0.77159949999999999</v>
       </c>
       <c r="C48" s="112">
         <f>parameters!G48</f>
@@ -7763,25 +8058,25 @@
       </c>
       <c r="D48" s="114">
         <f>parameters!H48</f>
-        <v>8.0000000000000002E-3</v>
+        <v>0.77159949999999999</v>
       </c>
       <c r="E48" s="114">
         <f>parameters!I48</f>
-        <v>2.55106728462327E-3</v>
+        <v>4.8441961560982842E-2</v>
       </c>
       <c r="F48" s="114">
         <f>parameters!J48</f>
-        <v>8.0000000000000002E-3</v>
+        <v>0.77159949999999999</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="5" t="str">
         <f>parameters!D49</f>
-        <v>Utility.age</v>
+        <v>Sens.joined.diag.LG</v>
       </c>
       <c r="B49" s="113">
         <f>parameters!E49</f>
-        <v>4.3200000000000001E-3</v>
+        <v>0.1469713333333334</v>
       </c>
       <c r="C49" s="112">
         <f>parameters!G49</f>
@@ -7789,25 +8084,25 @@
       </c>
       <c r="D49" s="114">
         <f>parameters!H49</f>
-        <v>4.3200000000000001E-3</v>
+        <v>0.1469713333333334</v>
       </c>
       <c r="E49" s="114">
         <f>parameters!I49</f>
-        <v>1.4285976793890307E-4</v>
+        <v>9.2270402973300605E-3</v>
       </c>
       <c r="F49" s="114">
         <f>parameters!J49</f>
-        <v>4.3200000000000001E-3</v>
+        <v>0.1469713333333334</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="5" t="str">
         <f>parameters!D50</f>
-        <v>Disutility.HG.St1.3</v>
+        <v>Spec.joined.diag</v>
       </c>
       <c r="B50" s="113">
         <f>parameters!E50</f>
-        <v>-0.08</v>
+        <v>0.99642799999999998</v>
       </c>
       <c r="C50" s="112">
         <f>parameters!G50</f>
@@ -7815,25 +8110,25 @@
       </c>
       <c r="D50" s="114">
         <f>parameters!H50</f>
-        <v>-0.08</v>
+        <v>0.99642799999999998</v>
       </c>
       <c r="E50" s="114">
         <f>parameters!I50</f>
-        <v>4.3368143838595594E-2</v>
+        <v>7.4593207402382552E-4</v>
       </c>
       <c r="F50" s="114">
         <f>parameters!J50</f>
-        <v>-0.08</v>
+        <v>0.99642799999999998</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="5" t="str">
         <f>parameters!D51</f>
-        <v>Disutility.HG.St4</v>
+        <v>Mort.TURBT</v>
       </c>
       <c r="B51" s="113">
         <f>parameters!E51</f>
-        <v>-0.18</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="C51" s="112">
         <f>parameters!G51</f>
@@ -7841,233 +8136,233 @@
       </c>
       <c r="D51" s="114">
         <f>parameters!H51</f>
-        <v>-0.18</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E51" s="114">
         <f>parameters!I51</f>
-        <v>6.1225614830958487E-2</v>
+        <v>2.55106728462327E-3</v>
       </c>
       <c r="F51" s="114">
         <f>parameters!J51</f>
-        <v>-0.18</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="5" t="str">
         <f>parameters!D52</f>
-        <v>Disutility.LG</v>
+        <v>Utility.age</v>
       </c>
       <c r="B52" s="113">
         <f>parameters!E52</f>
-        <v>0</v>
+        <v>4.3200000000000001E-3</v>
       </c>
       <c r="C52" s="112">
         <f>parameters!G52</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D52" s="114">
         <f>parameters!H52</f>
-        <v>0</v>
+        <v>4.3200000000000001E-3</v>
       </c>
       <c r="E52" s="114">
         <f>parameters!I52</f>
-        <v>0</v>
+        <v>1.4285976793890307E-4</v>
       </c>
       <c r="F52" s="114">
         <f>parameters!J52</f>
-        <v>0</v>
+        <v>4.3200000000000001E-3</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="5" t="str">
         <f>parameters!D53</f>
-        <v>Cost.diag.sympt</v>
+        <v>Disutility.HG.St1.3</v>
       </c>
       <c r="B53" s="113">
         <f>parameters!E53</f>
-        <v>610.58000000000004</v>
+        <v>-0.08</v>
       </c>
       <c r="C53" s="112">
         <f>parameters!G53</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D53" s="114">
         <f>parameters!H53</f>
-        <v>100</v>
+        <v>-0.08</v>
       </c>
       <c r="E53" s="114">
         <f>parameters!I53</f>
-        <v>6.1058000000000003</v>
+        <v>4.3368143838595594E-2</v>
       </c>
       <c r="F53" s="114">
         <f>parameters!J53</f>
-        <v>610.58000000000004</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="5" t="str">
         <f>parameters!D54</f>
-        <v>Cost.diag.screen</v>
+        <v>Disutility.HG.St4</v>
       </c>
       <c r="B54" s="113">
         <f>parameters!E54</f>
-        <v>584.89</v>
+        <v>-0.18</v>
       </c>
       <c r="C54" s="112">
         <f>parameters!G54</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D54" s="114">
         <f>parameters!H54</f>
-        <v>100</v>
+        <v>-0.18</v>
       </c>
       <c r="E54" s="114">
         <f>parameters!I54</f>
-        <v>5.8488999999999995</v>
+        <v>6.1225614830958487E-2</v>
       </c>
       <c r="F54" s="114">
         <f>parameters!J54</f>
-        <v>584.89</v>
+        <v>-0.18</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="5" t="str">
         <f>parameters!D55</f>
-        <v>Cost.treat.intercept</v>
+        <v>Disutility.LG</v>
       </c>
       <c r="B55" s="113">
         <f>parameters!E55</f>
-        <v>2348.8000000000002</v>
+        <v>0</v>
       </c>
       <c r="C55" s="112">
         <f>parameters!G55</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D55" s="114">
         <f>parameters!H55</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E55" s="114">
         <f>parameters!I55</f>
-        <v>23.488000000000003</v>
+        <v>0</v>
       </c>
       <c r="F55" s="114">
         <f>parameters!J55</f>
-        <v>2348.8000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="5" t="str">
         <f>parameters!D56</f>
-        <v>Cost.treat.past.smoke</v>
+        <v>Cost.diag.sympt</v>
       </c>
       <c r="B56" s="113">
         <f>parameters!E56</f>
-        <v>-57.2</v>
+        <v>612.14</v>
       </c>
       <c r="C56" s="112">
         <f>parameters!G56</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D56" s="114">
         <f>parameters!H56</f>
-        <v>-57.2</v>
+        <v>100</v>
       </c>
       <c r="E56" s="114">
         <f>parameters!I56</f>
-        <v>5.7200000000000006</v>
+        <v>6.1213999999999995</v>
       </c>
       <c r="F56" s="114">
         <f>parameters!J56</f>
-        <v>-57.2</v>
+        <v>612.14</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="5" t="str">
         <f>parameters!D57</f>
-        <v>Cost.treat.current.smoke</v>
+        <v>Cost.diag.screen1</v>
       </c>
       <c r="B57" s="113">
         <f>parameters!E57</f>
-        <v>-242</v>
+        <v>135.38999999999999</v>
       </c>
       <c r="C57" s="112">
         <f>parameters!G57</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D57" s="114">
         <f>parameters!H57</f>
-        <v>-242</v>
+        <v>100</v>
       </c>
       <c r="E57" s="114">
         <f>parameters!I57</f>
-        <v>24.200000000000003</v>
+        <v>1.3538999999999999</v>
       </c>
       <c r="F57" s="114">
         <f>parameters!J57</f>
-        <v>-242</v>
+        <v>135.38999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="5" t="str">
         <f>parameters!D58</f>
-        <v>Cost.treat.Y2</v>
+        <v>Cost.diag.screen2</v>
       </c>
       <c r="B58" s="113">
         <f>parameters!E58</f>
-        <v>-921.4</v>
+        <v>534.96</v>
       </c>
       <c r="C58" s="112">
         <f>parameters!G58</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D58" s="114">
         <f>parameters!H58</f>
-        <v>-921.4</v>
+        <v>100</v>
       </c>
       <c r="E58" s="114">
         <f>parameters!I58</f>
-        <v>92.14</v>
+        <v>5.3496000000000006</v>
       </c>
       <c r="F58" s="114">
         <f>parameters!J58</f>
-        <v>-921.4</v>
+        <v>534.96</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="5" t="str">
         <f>parameters!D59</f>
-        <v>Cost.treat.Y3</v>
+        <v>Cost.treat.intercept</v>
       </c>
       <c r="B59" s="113">
         <f>parameters!E59</f>
-        <v>-1514</v>
+        <v>2348.8000000000002</v>
       </c>
       <c r="C59" s="112">
         <f>parameters!G59</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D59" s="114">
         <f>parameters!H59</f>
-        <v>-1514</v>
+        <v>100</v>
       </c>
       <c r="E59" s="114">
         <f>parameters!I59</f>
-        <v>151.4</v>
+        <v>23.488000000000003</v>
       </c>
       <c r="F59" s="114">
         <f>parameters!J59</f>
-        <v>-1514</v>
+        <v>2348.8000000000002</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="5" t="str">
         <f>parameters!D60</f>
-        <v>Cost.treat.stage1</v>
+        <v>Cost.treat.past.smoke</v>
       </c>
       <c r="B60" s="113">
         <f>parameters!E60</f>
-        <v>1446.8</v>
+        <v>-57.2</v>
       </c>
       <c r="C60" s="112">
         <f>parameters!G60</f>
@@ -8075,25 +8370,25 @@
       </c>
       <c r="D60" s="114">
         <f>parameters!H60</f>
-        <v>1446.8</v>
+        <v>-57.2</v>
       </c>
       <c r="E60" s="114">
         <f>parameters!I60</f>
-        <v>144.68</v>
+        <v>5.7200000000000006</v>
       </c>
       <c r="F60" s="114">
         <f>parameters!J60</f>
-        <v>1446.8</v>
+        <v>-57.2</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="5" t="str">
         <f>parameters!D61</f>
-        <v>Cost.treat.stage2</v>
+        <v>Cost.treat.current.smoke</v>
       </c>
       <c r="B61" s="113">
         <f>parameters!E61</f>
-        <v>1676.1</v>
+        <v>-242</v>
       </c>
       <c r="C61" s="112">
         <f>parameters!G61</f>
@@ -8101,25 +8396,25 @@
       </c>
       <c r="D61" s="114">
         <f>parameters!H61</f>
-        <v>1676.1</v>
+        <v>-242</v>
       </c>
       <c r="E61" s="114">
         <f>parameters!I61</f>
-        <v>167.61</v>
+        <v>24.200000000000003</v>
       </c>
       <c r="F61" s="114">
         <f>parameters!J61</f>
-        <v>1676.1</v>
+        <v>-242</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="5" t="str">
         <f>parameters!D62</f>
-        <v>Cost.treat.stage3</v>
+        <v>Cost.treat.Y2</v>
       </c>
       <c r="B62" s="113">
         <f>parameters!E62</f>
-        <v>3956.7</v>
+        <v>-921.4</v>
       </c>
       <c r="C62" s="112">
         <f>parameters!G62</f>
@@ -8127,25 +8422,25 @@
       </c>
       <c r="D62" s="114">
         <f>parameters!H62</f>
-        <v>3956.7</v>
+        <v>-921.4</v>
       </c>
       <c r="E62" s="114">
         <f>parameters!I62</f>
-        <v>395.67</v>
+        <v>92.14</v>
       </c>
       <c r="F62" s="114">
         <f>parameters!J62</f>
-        <v>3956.7</v>
+        <v>-921.4</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="5" t="str">
         <f>parameters!D63</f>
-        <v>Cost.treat.stage4</v>
+        <v>Cost.treat.Y3</v>
       </c>
       <c r="B63" s="113">
         <f>parameters!E63</f>
-        <v>5406.9</v>
+        <v>-1514</v>
       </c>
       <c r="C63" s="112">
         <f>parameters!G63</f>
@@ -8153,25 +8448,25 @@
       </c>
       <c r="D63" s="114">
         <f>parameters!H63</f>
-        <v>5406.9</v>
+        <v>-1514</v>
       </c>
       <c r="E63" s="114">
         <f>parameters!I63</f>
-        <v>540.68999999999994</v>
+        <v>151.4</v>
       </c>
       <c r="F63" s="114">
         <f>parameters!J63</f>
-        <v>5406.9</v>
+        <v>-1514</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="5" t="str">
         <f>parameters!D64</f>
-        <v>Cost.treat.LG</v>
+        <v>Cost.treat.stage1</v>
       </c>
       <c r="B64" s="113">
         <f>parameters!E64</f>
-        <v>1217.4000000000001</v>
+        <v>1446.8</v>
       </c>
       <c r="C64" s="112">
         <f>parameters!G64</f>
@@ -8179,129 +8474,129 @@
       </c>
       <c r="D64" s="114">
         <f>parameters!H64</f>
-        <v>1217.4000000000001</v>
+        <v>1446.8</v>
       </c>
       <c r="E64" s="114">
         <f>parameters!I64</f>
-        <v>121.74000000000001</v>
+        <v>144.68</v>
       </c>
       <c r="F64" s="114">
         <f>parameters!J64</f>
-        <v>1217.4000000000001</v>
+        <v>1446.8</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="5" t="str">
         <f>parameters!D65</f>
-        <v>Cost.surv.Y4.5</v>
+        <v>Cost.treat.stage2</v>
       </c>
       <c r="B65" s="113">
         <f>parameters!E65</f>
-        <v>401</v>
+        <v>1676.1</v>
       </c>
       <c r="C65" s="112">
         <f>parameters!G65</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D65" s="114">
         <f>parameters!H65</f>
-        <v>100</v>
+        <v>1676.1</v>
       </c>
       <c r="E65" s="114">
         <f>parameters!I65</f>
-        <v>4.01</v>
+        <v>167.61</v>
       </c>
       <c r="F65" s="114">
         <f>parameters!J65</f>
-        <v>401</v>
+        <v>1676.1</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="5" t="str">
         <f>parameters!D66</f>
-        <v>Cost.dipstick.invite</v>
+        <v>Cost.treat.stage3</v>
       </c>
       <c r="B66" s="113">
         <f>parameters!E66</f>
-        <v>8.57</v>
+        <v>3956.7</v>
       </c>
       <c r="C66" s="112">
         <f>parameters!G66</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D66" s="114">
         <f>parameters!H66</f>
-        <v>100</v>
+        <v>3956.7</v>
       </c>
       <c r="E66" s="114">
         <f>parameters!I66</f>
-        <v>8.5699999999999998E-2</v>
+        <v>395.67</v>
       </c>
       <c r="F66" s="114">
         <f>parameters!J66</f>
-        <v>8.57</v>
+        <v>3956.7</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="5" t="str">
         <f>parameters!D67</f>
-        <v>Cost.ad.dipstick</v>
+        <v>Cost.treat.stage4</v>
       </c>
       <c r="B67" s="113">
         <f>parameters!E67</f>
-        <v>1.3</v>
+        <v>5406.9</v>
       </c>
       <c r="C67" s="112">
         <f>parameters!G67</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D67" s="114">
         <f>parameters!H67</f>
-        <v>100</v>
+        <v>5406.9</v>
       </c>
       <c r="E67" s="114">
         <f>parameters!I67</f>
-        <v>1.3000000000000001E-2</v>
+        <v>540.68999999999994</v>
       </c>
       <c r="F67" s="114">
         <f>parameters!J67</f>
-        <v>1.3</v>
+        <v>5406.9</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="5" t="str">
         <f>parameters!D68</f>
-        <v>Cost.dipstick.positive</v>
+        <v>Cost.treat.LG</v>
       </c>
       <c r="B68" s="113">
         <f>parameters!E68</f>
-        <v>11.8</v>
+        <v>1217.4000000000001</v>
       </c>
       <c r="C68" s="112">
         <f>parameters!G68</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D68" s="114">
         <f>parameters!H68</f>
-        <v>100</v>
+        <v>1217.4000000000001</v>
       </c>
       <c r="E68" s="114">
         <f>parameters!I68</f>
-        <v>0.11800000000000001</v>
+        <v>121.74000000000001</v>
       </c>
       <c r="F68" s="114">
         <f>parameters!J68</f>
-        <v>11.8</v>
+        <v>1217.4000000000001</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="5" t="str">
         <f>parameters!D69</f>
-        <v>Cost.dipstick</v>
+        <v>Cost.surv.Y4.5</v>
       </c>
       <c r="B69" s="113">
         <f>parameters!E69</f>
-        <v>3.86</v>
+        <v>401</v>
       </c>
       <c r="C69" s="112">
         <f>parameters!G69</f>
@@ -8313,28 +8608,124 @@
       </c>
       <c r="E69" s="114">
         <f>parameters!I69</f>
-        <v>3.8599999999999995E-2</v>
+        <v>4.01</v>
       </c>
       <c r="F69" s="114">
         <f>parameters!J69</f>
+        <v>401</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="5" t="str">
+        <f>parameters!D70</f>
+        <v>Cost.dipstick.invite</v>
+      </c>
+      <c r="B70" s="113">
+        <f>parameters!E70</f>
+        <v>8.57</v>
+      </c>
+      <c r="C70" s="112">
+        <f>parameters!G70</f>
+        <v>2</v>
+      </c>
+      <c r="D70" s="114">
+        <f>parameters!H70</f>
+        <v>100</v>
+      </c>
+      <c r="E70" s="114">
+        <f>parameters!I70</f>
+        <v>8.5699999999999998E-2</v>
+      </c>
+      <c r="F70" s="114">
+        <f>parameters!J70</f>
+        <v>8.57</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="5" t="str">
+        <f>parameters!D71</f>
+        <v>Cost.ad.dipstick</v>
+      </c>
+      <c r="B71" s="113">
+        <f>parameters!E71</f>
+        <v>1.3</v>
+      </c>
+      <c r="C71" s="112">
+        <f>parameters!G71</f>
+        <v>2</v>
+      </c>
+      <c r="D71" s="114">
+        <f>parameters!H71</f>
+        <v>100</v>
+      </c>
+      <c r="E71" s="114">
+        <f>parameters!I71</f>
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="F71" s="114">
+        <f>parameters!J71</f>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="5" t="str">
+        <f>parameters!D72</f>
+        <v>Cost.dipstick.positive</v>
+      </c>
+      <c r="B72" s="113">
+        <f>parameters!E72</f>
+        <v>11.8</v>
+      </c>
+      <c r="C72" s="112">
+        <f>parameters!G72</f>
+        <v>2</v>
+      </c>
+      <c r="D72" s="114">
+        <f>parameters!H72</f>
+        <v>100</v>
+      </c>
+      <c r="E72" s="114">
+        <f>parameters!I72</f>
+        <v>0.11800000000000001</v>
+      </c>
+      <c r="F72" s="114">
+        <f>parameters!J72</f>
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="5" t="str">
+        <f>parameters!D73</f>
+        <v>Cost.dipstick</v>
+      </c>
+      <c r="B73" s="113">
+        <f>parameters!E73</f>
         <v>3.86</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="5"/>
-      <c r="B70" s="113"/>
-      <c r="C70" s="112"/>
-      <c r="D70" s="114"/>
-      <c r="E70" s="114"/>
-      <c r="F70" s="114"/>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="5"/>
-      <c r="B71" s="110"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="110"/>
-      <c r="E71" s="110"/>
-      <c r="F71" s="110"/>
+      <c r="C73" s="112">
+        <f>parameters!G73</f>
+        <v>2</v>
+      </c>
+      <c r="D73" s="114">
+        <f>parameters!H73</f>
+        <v>100</v>
+      </c>
+      <c r="E73" s="114">
+        <f>parameters!I73</f>
+        <v>3.8599999999999995E-2</v>
+      </c>
+      <c r="F73" s="114">
+        <f>parameters!J73</f>
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="5"/>
+      <c r="B74" s="113"/>
+      <c r="C74" s="112"/>
+      <c r="D74" s="114"/>
+      <c r="E74" s="114"/>
+      <c r="F74" s="114"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -8367,8 +8758,8 @@
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
       <c r="J1" s="8"/>
-      <c r="K1" s="118"/>
-      <c r="L1" s="119"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="124"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="7"/>
@@ -8423,21 +8814,21 @@
       <c r="A6" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="120" t="s">
+      <c r="B6" s="125" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="120"/>
-      <c r="D6" s="120"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="120"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
       <c r="G6" s="15"/>
-      <c r="H6" s="120" t="s">
+      <c r="H6" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="I6" s="120"/>
-      <c r="J6" s="120"/>
-      <c r="K6" s="120"/>
-      <c r="L6" s="120"/>
+      <c r="I6" s="125"/>
+      <c r="J6" s="125"/>
+      <c r="K6" s="125"/>
+      <c r="L6" s="125"/>
     </row>
     <row r="7" spans="1:12" ht="18.75">
       <c r="A7" s="16" t="s">
@@ -12389,13 +12780,13 @@
       <c r="P1" s="66" t="s">
         <v>158</v>
       </c>
-      <c r="R1" s="121" t="s">
+      <c r="R1" s="126" t="s">
         <v>115</v>
       </c>
-      <c r="S1" s="119"/>
-      <c r="T1" s="119"/>
-      <c r="U1" s="119"/>
-      <c r="V1" s="119"/>
+      <c r="S1" s="124"/>
+      <c r="T1" s="124"/>
+      <c r="U1" s="124"/>
+      <c r="V1" s="124"/>
       <c r="W1">
         <v>100000</v>
       </c>
@@ -19278,20 +19669,20 @@
       <c r="L1" s="71" t="s">
         <v>170</v>
       </c>
-      <c r="N1" s="122" t="s">
+      <c r="N1" s="127" t="s">
         <v>171</v>
       </c>
-      <c r="O1" s="122"/>
-      <c r="P1" s="122"/>
-      <c r="Q1" s="122"/>
-      <c r="R1" s="122"/>
-      <c r="S1" s="122"/>
-      <c r="T1" s="122"/>
-      <c r="U1" s="122"/>
-      <c r="V1" s="122"/>
-      <c r="W1" s="122"/>
-      <c r="X1" s="122"/>
-      <c r="Y1" s="122"/>
+      <c r="O1" s="127"/>
+      <c r="P1" s="127"/>
+      <c r="Q1" s="127"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="127"/>
+      <c r="T1" s="127"/>
+      <c r="U1" s="127"/>
+      <c r="V1" s="127"/>
+      <c r="W1" s="127"/>
+      <c r="X1" s="127"/>
+      <c r="Y1" s="127"/>
     </row>
     <row r="2" spans="1:35" ht="46.5" customHeight="1">
       <c r="A2" s="72" t="s">
@@ -19330,14 +19721,14 @@
       <c r="L2" s="74">
         <v>100.5</v>
       </c>
-      <c r="N2" s="122" t="s">
+      <c r="N2" s="127" t="s">
         <v>180</v>
       </c>
-      <c r="O2" s="122"/>
-      <c r="P2" s="122"/>
-      <c r="Q2" s="122"/>
-      <c r="R2" s="122"/>
-      <c r="S2" s="122"/>
+      <c r="O2" s="127"/>
+      <c r="P2" s="127"/>
+      <c r="Q2" s="127"/>
+      <c r="R2" s="127"/>
+      <c r="S2" s="127"/>
       <c r="T2" s="75"/>
       <c r="U2" s="75"/>
       <c r="V2" s="76"/>
@@ -31790,14 +32181,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" hidden="1">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="127" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
     </row>
     <row r="2" spans="1:13">
       <c r="B2" s="67" t="str">
@@ -34757,4 +35148,253 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453BC69A-9797-41D2-A7DC-4E7350C17670}">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="8" width="16.5703125" style="116" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="36.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="D1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E1" t="s">
+        <v>346</v>
+      </c>
+      <c r="G1" t="s">
+        <v>345</v>
+      </c>
+      <c r="H1" s="116" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B2">
+        <v>2016</v>
+      </c>
+      <c r="C2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D2">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="E2">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="F2" s="116">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="G2" s="116">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="H2" s="116">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="I2">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="J2" s="118" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B3">
+        <v>2011</v>
+      </c>
+      <c r="C3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D3">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="E3">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="F3" s="116">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="G3" s="116">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="H3" s="116">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="I3">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="J3" s="118" t="s">
+        <v>348</v>
+      </c>
+      <c r="L3" s="116"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="L4" s="116"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>351</v>
+      </c>
+      <c r="D5">
+        <f>D2*D3</f>
+        <v>0.44091399999999997</v>
+      </c>
+      <c r="E5" s="116">
+        <f>E2*E3</f>
+        <v>0.38762400000000002</v>
+      </c>
+      <c r="F5" s="116">
+        <f>F2*F3</f>
+        <v>0.49613200000000002</v>
+      </c>
+      <c r="G5" s="116">
+        <f>1-(1-G2)*(1-G3)</f>
+        <v>0.99642799999999998</v>
+      </c>
+      <c r="H5" s="116">
+        <f>1-(1-H2)*(1-H3)</f>
+        <v>0.99468900000000005</v>
+      </c>
+      <c r="I5" s="116">
+        <f>1-(1-I2)*(1-I3)</f>
+        <v>0.99761299999999997</v>
+      </c>
+      <c r="L5" s="116"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="E6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>361</v>
+      </c>
+      <c r="B7">
+        <v>2015</v>
+      </c>
+      <c r="C7" t="s">
+        <v>360</v>
+      </c>
+      <c r="D7">
+        <v>0.84</v>
+      </c>
+      <c r="E7">
+        <f>(D7)*100/$D$9-100</f>
+        <v>75</v>
+      </c>
+      <c r="J7" s="118" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="C8" t="s">
+        <v>359</v>
+      </c>
+      <c r="D8">
+        <v>0.16</v>
+      </c>
+      <c r="E8" s="119">
+        <f>(D8)*100/$D$9-100</f>
+        <v>-66.666666666666657</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="C9" t="s">
+        <v>362</v>
+      </c>
+      <c r="D9">
+        <v>0.48</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="C11" s="119" t="s">
+        <v>365</v>
+      </c>
+      <c r="D11">
+        <f>D$5+D$5*$E$7/100</f>
+        <v>0.77159949999999999</v>
+      </c>
+      <c r="E11" s="119">
+        <f t="shared" ref="E11:F11" si="0">E$5+E$5*$E$7/100</f>
+        <v>0.678342</v>
+      </c>
+      <c r="F11" s="119">
+        <f t="shared" si="0"/>
+        <v>0.86823100000000009</v>
+      </c>
+      <c r="G11" s="116">
+        <f>G2</f>
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="H11" s="119">
+        <f t="shared" ref="H11:I12" si="1">H2</f>
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="I11" s="119">
+        <f t="shared" si="1"/>
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="C12" s="119" t="s">
+        <v>364</v>
+      </c>
+      <c r="D12" s="119">
+        <f>D$5+D$5*$E$8/100</f>
+        <v>0.1469713333333334</v>
+      </c>
+      <c r="E12" s="119">
+        <f t="shared" ref="E12:F12" si="2">E$5+E$5*$E$8/100</f>
+        <v>0.12920800000000005</v>
+      </c>
+      <c r="F12" s="119">
+        <f t="shared" si="2"/>
+        <v>0.16537733333333338</v>
+      </c>
+      <c r="G12" s="119">
+        <f>G3</f>
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="H12" s="119">
+        <f t="shared" si="1"/>
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="I12" s="119">
+        <f t="shared" si="1"/>
+        <v>0.96899999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{E75905EB-5EFF-454F-994B-2B716CDFAF98}"/>
+    <hyperlink ref="J3" r:id="rId2" tooltip="Persistent link using digital object identifier" xr:uid="{7E9C84DA-018A-4C49-9AB4-B46E9122F1B8}"/>
+    <hyperlink ref="J7" r:id="rId3" tooltip="Persistent link using digital object identifier" xr:uid="{A1150F4E-3A25-4772-94AB-FB76F6D30322}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>